<commit_message>
Excel Updated: 30th 5:10
</commit_message>
<xml_diff>
--- a/Master Excel.xlsx
+++ b/Master Excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Documents\Kijiji Ad Reposter\Kijiji-Ad-Reposter-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981463EC-D2C7-40AE-8BC5-26E529360866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C9416B-9F88-4B82-AE55-D79C6EB9BD58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{393D3522-DE12-4350-BF0C-774FF81A8306}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{393D3522-DE12-4350-BF0C-774FF81A8306}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -9796,100 +9796,6 @@
 WEEKENDS: 10AM - 7PM</t>
   </si>
   <si>
-    <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
-Best Price, Best Quality
-Buy with Confidence from our store! ✨
-----------------------------------------------------
-CELLULAR + WIFI
-----------------------------------------------------
-Samsung Tab S9 FE 5G (Wi-Fi + LTE)
-(OPEN BOX WITH WARRANTY)
-- 10.9" Display
-- 128GB Storage
-Price - $495 (CASH NO TAX)
------------------------------------------------------
-WIFI
------------------------------------------------------
-Samsung Galaxy Tab S9 Ultra 14.6" 512GB Android Tablet with Snapdragon Gen 2 Processor (CANADIAN MODEL)
-(BRAND NEW IN BOX WITH 1 YEAR SAMSUNG WARRANTY)
-- 14.6" Display
-- 512GB Stоrage
-- 12GB RAM
-Price - $1195 (CASH NО TAX)
-Samsung Galaxy Tab S9 ULTRA (Wi-Fi) With Keyboard Case (which is worth $150 for Free)(International Model)
-(BRAND NEW IN BOX WITH 1-Year WARRANTY)
-- 14.6" Display
-- 512GB Storage
-- 12GB RAM
-Price - $1195 (CASH NO TAX)
-Samsung Galaxy Tab S9 ULTRA (Wi-Fi) With Keyboard Case (which is worth $150 for Free)(International Model)
-(BRAND NEW IN BOX WITH 1-Year WARRANTY)
-- 14.6" Display
-- 256GB Storage
-- 12GB RAM
-Price - $1095 (CASH NO TAX)
-----------------------------------------------------
-Samsung Galaxy Tab S9+ (Wi-Fi) X810 with Kеyboard Case (which is worth $150 for Frеe)(International Model)
-(BRAND NEW IN BOX WITH 1 YEAR Warranty )
--12.4' Display
-- 512GB Storage
-- 12GB RAM
-Price - $1045 (CASH NO TAX)
-----------------------------------------------------
-Samsung Tab S9 FE+ (WiFi)
-(BRAND NEW IN BOX WITH WARRANTY)
-- 12.4" Display
-- 256GB Storage
-- 12GB RAM
-Price - $695 (CASH NO TAX)
-----------------------------------------------------
-Samsung Tab S9 FE (WiFi)
-(BRAND NEW IN BOX WITH WARRANTY)
-- 10.9" Display
-- 128GB Storage
-- 6GB RAM
-Price - $395 (CASH NO TAX)
-----------------------------------------------------
-Samsung Galaxy Tab S6 Lite P613 (Wi-Fi)
-(BRAND NEW IN BOX WITH 1 YEAR WARRANTY)
-- 10.4" Display
-- 128GB Storage
-- 4GB RAM
-Price - $345(CASH NO TAX)
-Samsung Galaxy Tab S6 Lite P613 (Wi-Fi)
-(BRAND NEW IN BOX WITH 1 YEAR SAMSUNG WARRANTY)
-- 10.4" Display
-- 64GB Stоrage
-- 4GB RAM
-Price - $325(CASH NO TAX)
-----------------------------------------------------
-Same day delivery available in GTA area -delivery charges are extra depends on location
-----------------------------------------------------
-BUY NOW. PAY LATER.
-Get easy monthly financing when you shop with Canadian Outlet
-Split your purchase into stress-free, automatic installments with monthly Plans for :-
-3 Months
-6 Months
-12 Months
-*All financing done through Pay Bright
-----------------------------------------------------
-Storefront is open to public 7 days a week
-----------------------------------------------------
-We are providing a FREE parking facility for our customers (Contact us)!!
-----------------------------------------------------
-STORE LOCATION:
-CANADIAN OUTLET
-1431 YONGE STREET
-YONGE &amp; ST СLAIR
-TORONTO, ON
-M4T 1Y7
-647 786 4344 (MAIN NUMBER)
-4164744786
-TIMINGS:
-MONDAY - FRIDAY: 8AM - 8PM
-WEEKENDS: 10AM - 7PM</t>
-  </si>
-  <si>
     <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choicе!
 Best Price, Best Quality
 Buy with Confidence from our store! ✨
@@ -11665,6 +11571,1808 @@
     <t>Elgato Streaming - Elgato HD60X, HD60S, Facecam</t>
   </si>
   <si>
+    <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
+Best Price, Best Quality
+Buy with Confidence from our store! ✨
+---------------------------------------------
+Samsung Phones - Samsung Galaxy A73, Samsung Galaxy A72, Samsung Galaxy A71, Samsung Galaxy A55, Samsung Galaxy A54, Samsung Galaxy A53, Samsung Galaxy A52s, Samsung Galaxy A52, Samsung Galaxy A51 Phone, Samsung A50
+BLOWOUT SALE!!!
+---------------------------------------------
+Samsung Galaxy A73 128GB/6GB RAM (Dual Sim)
+(Brand New In Box With Warranty)
+Pricе: $545 (Cash No Tax)
+Samsung Galaxy A72 256GB/8GB RAM (Dual Sim)
+(Brand New In Box With Wаrranty)
+Price: $540 (Cash No Tax)
+---------------------------------------------
+Samsung Galaxy A71 5G 128GB/ 6GB RAM
+(Fully Functional With store Warranty)
+Price: $195 (Cash Nо Tax)
+------------------------------------------------------------------
+Samsung Galaxy A55 5G 128GB (DUAL SIM)
+(Brand New In Box With Warranty)
+Price: $470 (Cash No Tax)
+------------------------------------------------------------------
+Samsung Galaxy A54 5G 128GB (Canadiаn / US Model)
+(Brand New In Box With Warranty)
+Price: $395 (Cash No Tax)
+Samsung Galaxy A54 5G 128GB
+(New In Box With Warranty)
+Price: $370 (Cash No Tax)
+------------------------------------------------------------------
+Samsung Galaxy A53 5G 128GB
+(New In Box With Warranty)
+Price: $360 (Cash No Tax)
+------------------------------------------------------
+Samsung Galaxy A52s 5G 128GB
+(Like New in Box With Warranty)
+Price: $275 (Cash No Tax)
+------------------------------------------------------
+Samsung Galaxy A52 5G 128GB
+(New in Box With Warranty)
+Price: $250 (Cash No Tax)
+------------------------------------------------------------------
+Samsung Galaxy A51 5G 128GB
+(Like New in Box With Warranty)
+Price: $195 (Cash No Tax)
+Samsung Galаxy A51 128GB
+(Like New in Box With Warranty)
+Price: $175 (Cash No Tax)
+Samsung Galaxy A51 64GB
+(Like New in Box With Warranty)
+Price: $150 (Cash No Tax)
+------------------------------------------------------------------
+Samsung Galaxy A50 64GB
+(Like New In Box With Warranty)
+Price: $175 (Cash No Tax)
+------------------------------------------------------------------
+Same day delivery available in GTA area -delivery charges are extra depends on location
+------------------------------------------------------------------
+BUY NOW. PAY LАTER.
+Get easy monthly financing when you shoр with Canadian Outlet
+Split your purchase into stress-free, automatic installments with monthly Plans for:-
+3 Months
+6 Months
+12 Months
+*All financing done through Pay Bright
+-------------------------------------------------------------------
+Storefront is open to public 7 days a week
+-------------------------------------------------------------------
+We are providing FREE parking facility for our customers (Contаct us)!!
+-------------------------------------------------------------------
+STORE LOCATION:
+CANADIAN OUTLET
+1431 YONGE STREET
+YONGE &amp; ST CLAIR
+TORONTO, ON
+M4T 1Y7
+647 786 4344 (MАIN NUMBER)
+4164744786
+TIMINGS:
+MONDAY - FRIDAY: 8AM - 8PM
+WEEKENDS: 10AM - 7PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
+Best Price, Best Quality 
+Buy with Confidence from our store! ✨
+------------------------------------------------------
+Arctic King Window Air Conditioner - 10000 BTU - 450 sq ft (MWHUK10CRN8BCL0)
+(BRAND NEW IN BOX WITH 1 YEAR MANUFACTURER WARRANTY)
+REGULAR PRICE: $469 + TAX
+OUR PRICE: $375 (CASH NO TAX)
+------------------------------------------------------
+BUY NOW. PAY LATER.
+Get easy monthly financing when you shop with Canadian Outlet
+Split your purchase into stress-free, automatic installments with monthly Plans for:-
+3 Months
+6 Months
+12 Months
+*All financing done through Pay Bright
+------------------------------------------------------
+Same day delivery available in GTA area - delivery charges are extra depends on location
+------------------------------------------------------
+Storefront is open to public 7 days a week
+------------------------------------------------------
+We are providing FREE parking facility for our customers (Contact us)!!
+------------------------------------------------------
+STORE LOCATION:
+CANADIAN OUTLET
+1431 YONGE STREET
+YONGE &amp; ST CLAIR
+TORONTO, ON
+M4T 1Y7
+647 786 4344 (MAIN NUMBER)
+416 474 4786
+TIMINGS:
+MONDAY - FRIDAY: 8AM - 8PM
+WEEKENDS: 10AM - 7PM
+</t>
+  </si>
+  <si>
+    <t>Arctic King Window AC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8000 BTU Air Conditioners - Arctic King, OmniMax, Forest Air </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
+Best Price, Best Quality 
+Buy with Confidence from our store! ✨
+------------------------------------------------------
+Forest Air 3-in-1 Portable Air Conditioner - 8000 BTU - 200-250 sq ft (A01908KR)
+(BRAND NEW IN BOX WITH 1 YEAR MANUFACTURER WARRANTY)
+REGULAR PRICE: $445.50 + TAX
+OUR PRICE: $345 (CASH NO TAX)
+------------------------------------------------------
+OMNIMAX 3-in-1 Portable Air Conditioner - 8000 BTU - 150 sq ft (OP08N3WBA1RCM)
+(BRAND NEW IN BOX WITH 1 YEAR MANUFACTURER WARRANTY)
+REGULAR PRICE: $449.99 + TAX
+OUR PRICE: $345 (CASH NO TAX)
+------------------------------------------------------
+Arctic King Portable Air Conditioner - 8000 BTU - 150 sq ft (AP53SEWBA1RCM)
+(BRAND NEW IN BOX WITH 1 YEAR MANUFACTURER WARRANTY)
+REGULAR PRICE: $379 + TAX
+OUR PRICE: $325 (CASH NO TAX)
+------------------------------------------------------
+BUY NOW. PAY LATER.
+Get easy monthly financing when you shop with Canadian Outlet
+Split your purchase into stress-free, automatic installments with monthly Plans for:-
+3 Months
+6 Months
+12 Months
+*All financing done through Pay Bright
+------------------------------------------------------
+Same day delivery available in GTA area - delivery charges are extra depends on location
+------------------------------------------------------
+Storefront is open to public 7 days a week
+------------------------------------------------------
+We are providing FREE parking facility for our customers (Contact us)!!
+------------------------------------------------------
+STORE LOCATION:
+CANADIAN OUTLET
+1431 YONGE STREET
+YONGE &amp; ST CLAIR
+TORONTO, ON
+M4T 1Y7
+647 786 4344 (MAIN NUMBER)
+416 474 4786
+TIMINGS:
+MONDAY - FRIDAY: 8AM - 8PM
+WEEKENDS: 10AM - 7PM
+</t>
+  </si>
+  <si>
+    <t>8000 BTU AC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
+Best Price, Best Quality 
+Buy with Confidence from our store! ✨
+------------------------------------------------------
+Arctic King Portable Air Conditioner - 10000 BTU - 300 sq ft (AP07SEWBA1RCM) 
+(BRAND NEW IN BOX WITH 1 YEAR MANUFACTURER WARRANTY)
+REGULAR PRICE: $549 + TAX
+OUR PRICE: $395 (CASH NO TAX)
+------------------------------------------------------
+KOOLKING Portable Air Conditioner - 10000 BTU - 540 sq ft
+(BRAND NEW IN BOX WITH 1 YEAR MANUFACTURER WARRANTY)
+REGULAR PRICE: $499.99 + TAX
+OUR PRICE: $395 (CASH NO TAX)
+------------------------------------------------------
+BUY NOW. PAY LATER.
+Get easy monthly financing when you shop with Canadian Outlet
+Split your purchase into stress-free, automatic installments with monthly Plans for:-
+3 Months
+6 Months
+12 Months
+*All financing done through Pay Bright
+------------------------------------------------------
+Same day delivery available in GTA area - delivery charges are extra depends on location
+------------------------------------------------------
+Storefront is open to public 7 days a week
+------------------------------------------------------
+We are providing FREE parking facility for our customers (Contact us)!!
+------------------------------------------------------
+STORE LOCATION:
+CANADIAN OUTLET
+1431 YONGE STREET
+YONGE &amp; ST CLAIR
+TORONTO, ON
+M4T 1Y7
+647 786 4344 (MAIN NUMBER)
+416 474 4786
+TIMINGS:
+MONDAY - FRIDAY: 8AM - 8PM
+WEEKENDS: 10AM - 7PM
+</t>
+  </si>
+  <si>
+    <t>10000 BTU AC</t>
+  </si>
+  <si>
+    <t>Arctic King, Hisense Air Conditioner - 13500 BTU, 13000BTU, 12000BTU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
+Best Price, Best Quality 
+Buy with Confidence from our store! ✨
+------------------------------------------------------
+Arctic King 3-in-1 Portable Air Conditioner - 13500 BTU - 450 sq ft (AP10SEWBA1RCM)
+(BRAND NEW IN BOX WITH 1 YEAR MANUFACTURER WARRANTY)
+REGULAR PRICE: $689 + TAX
+OUR PRICE: $545 (CASH NO TAX)
+------------------------------------------------------
+Hisense 3-in-1 Portable Smart Air Conditioner - 13000 BTU - 450 sq ft (AP1022CW1G)
+(BRAND NEW IN BOX WITH 1 YEAR MANUFACTURER WARRANTY)
+REGULAR PRICE: $697 + TAX
+OUR PRICE: $545 (CASH NO TAX)
+------------------------------------------------------
+Arctic King 3-in-1 Portable Air Conditioner - 12000 BTU - 350 sq ft (AP08SEWBA1RCM)
+(BRAND NEW IN BOX WITH 1 YEAR MANUFACTURER WARRANTY)
+REGULAR PRICE: $649 + TAX
+OUR PRICE: $495 (CASH NO TAX)
+------------------------------------------------------
+BUY NOW. PAY LATER.
+Get easy monthly financing when you shop with Canadian Outlet
+Split your purchase into stress-free, automatic installments with monthly Plans for:-
+3 Months
+6 Months
+12 Months
+*All financing done through Pay Bright
+------------------------------------------------------
+Same day delivery available in GTA area - delivery charges are extra depends on location
+------------------------------------------------------
+Storefront is open to public 7 days a week
+------------------------------------------------------
+We are providing FREE parking facility for our customers (Contact us)!!
+------------------------------------------------------
+STORE LOCATION:
+CANADIAN OUTLET
+1431 YONGE STREET
+YONGE &amp; ST CLAIR
+TORONTO, ON
+M4T 1Y7
+647 786 4344 (MAIN NUMBER)
+416 474 4786
+TIMINGS:
+MONDAY - FRIDAY: 8AM - 8PM
+WEEKENDS: 10AM - 7PM
+</t>
+  </si>
+  <si>
+    <t>High BTU AC</t>
+  </si>
+  <si>
+    <t>Samsung Phones - Samsung Z Fold 5, Fold 4, 3, 2, Flip 5, 4, 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
+Best Price, Best Quality 
+Buy with Confidence from our store! ✨
+---------------------------------------------------
+Ecohouzng Tower Air Cooler with Humidity - 3-Speed - 41-in - (#CT500032HF)
+(LIKE NEW WITH WARRANTY)
+OUR PRICE: $95 (CASH NO TAX)
+---------------------------------------------------
+BUY NOW. PAY LATER.
+Get easy monthly financing when you shop with Canadian Outlet
+Split your purchase into stress-free, automatic installments with monthly Plans for:-
+3 Months
+6 Months
+12 Months
+*All financing done through Pay Bright
+------------------------------------------------------
+Same day delivery available in GTA area - delivery charges are extra depends on location
+------------------------------------------------------
+Storefront is open to public 7 days a week
+------------------------------------------------------
+We are providing FREE parking facility for our customers (Contact us)!!
+------------------------------------------------------
+STORE LOCATION:
+CANADIAN OUTLET
+1431 YONGE STREET
+YONGE &amp; ST CLAIR
+TORONTO, ON
+M4T 1Y7
+647 786 4344 (MAIN NUMBER)
+416 474 4786
+TIMINGS:
+MONDAY - FRIDAY: 8AM - 8PM
+WEEKENDS: 10AM - 7PM
+</t>
+  </si>
+  <si>
+    <t>Ecohouzng Air Cooler</t>
+  </si>
+  <si>
+    <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
+Best Price, Best Quality 
+Buy with Confidence from our store!
+---------------------------------------------
+Fitbit Watches - Fitbit Charge 2, Fitbit Sense 2, Fitbit Sense, Fitbit Versa, Fitbit Inspire 2, Fitbit Charge 5 Fitness Tracker, Fitbit Charge 6 Fitness Tracker, Fitbit Luxe, Fitbit Versa 2, Fitbit Versa 3 Health &amp; Fitness Smartwatch, Fitbit Versa 1
+BLOWOUT SALE!!!
+-------------------------------------------------------------
+Fitbit Sense 2 Smartwatch
+(BRAND NEW WITH 1 YEAR FITBIT WARRANTY)
+PRICE - $225 (CASH NO TAX)
+Fitbit Sense Smartwatch
+(LIKE NEW WITH WARRANTY)
+PRICE - $125 (CASH NO TAX)
+-------------------------------------------------------------
+Fitbit Versa 4 Smartwatch
+(BRAND NEW WITH 1 YEAR FITBIT WARRANTY)
+PRICE - $175 (CASH NO TAX)
+Fitbit Versa 4 Smartwatch
+(LIKE NEW WITH WARRANTY)
+PRICE - $125 (CASH NO TAX)
+Fitbit Versa 3 Health &amp; Fitness Smartwatch
+(LIKE NEW WITH WARRANTY)
+PRICE - $140 (CASH NO TAX)
+Fitbit Versa 2 Smartwatch
+(LIKE NEW WITH WARRANTY)
+PRICE - $115 (CASH NO TAX)
+Fitbit Versa Smartwatch
+(LIKE NEW WITH WARRANTY)
+PRICE - $70 (CASH NO TAX)
+-------------------------------------------------------------
+Fitbit Charge 6 Fitness Tracker
+(LIKE NEW WITH WARRANTY)
+PRICE - $130 (CASH NO TAX)
+Fitbit Charge 5 Fitness Tracker
+(BRAND NEW IN BOX WITH WARRANTY)
+PRICE - $125(CASH NO TAX)
+Fitbit Charge 4 Fitness Tracker
+(LIKE NEW WITH WARRANTY)
+PRICE - $115 (CASH NO TAX)
+Fitbit Charge 2 Fitness Tracker
+(LIKE NEW WITH WARRANTY)
+PRICE - $55 (CASH NO TAX)
+-------------------------------------------------------------
+Fitbit Luxe Fitness and Wellness Tracker
+(LIKE NEW WITH WARRANTY)
+PRICE - $75 (CASH NO TAX)
+-------------------------------------------------------------
+Fitbit Inspire 2 Fitness Tracker with 24/7 Heart Rate 
+(BRAND NEW WITH 1 YEAR FITBIT WARRANTY)
+PRICE - $65 (CASH NO TAX)
+-------------------------------------------------------------
+Same day delivery available in GTA area - delivery charges are extra depends on location
+----------------------------------------------------
+BUY NOW. PAY LATER.
+Get easy monthly financing when you shop with Canadian Outlet
+Split your purchase into stress-free, automatic installments with monthly Plans for:-
+3 Months
+6 Months
+12 Months
+*All financing done through Pay Bright
+-------------------------------------------------------------------
+Storefront is open to public 7 days a week
+-------------------------------------------------------------------
+We are providing FREE parking facility for our customers (Contact us)!!
+-------------------------------------------------------------------
+STORE LOCATION:
+CANADIAN OUTLET
+1431 YONGE STREET
+YONGE &amp; ST CLAIR
+TORONTO, ON
+M4T 1Y7
+647 786 4344 (MAIN NUMBER)
+416 474 4786
+TIMINGS:
+MONDAY - FRIDAY: 8AM - 8PM
+WEEKENDS: 10AM - 7PM</t>
+  </si>
+  <si>
+    <t>JBL Speakers - JBL Clip 4, JBL Flip 6, JBL Charge 5</t>
+  </si>
+  <si>
+    <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
+Best Price, Best Quality
+Buy with Confidence from our store! ✨
+---------------------------------------------
+JBL Bluetooth Speakers - JBL Charge 5, JBL Flip 6, JBL Clip 4 Bluetooth Speakers
+----------------------------------------------------
+JBL Charge 5 Waterproof Bluetooth Wireless Speaker
+(BRAND NEW IN BOX WITH WARRANTY)
+Price - $185 (CASH NO TАX)
+JBL Flip 6 Waterproof Bluetooth Wirelеss Speaker
+(BRAND NEW IN BOX WITH WARRANTY)
+Price - $135 (CASH NO TAX)
+JBL Clip 4 Waterproof Bluetooth Wireless Speaker
+(BRAND NEW IN BOX WITH WARRANTY)
+Price - $75 (CASH NO TAX)
+------------------------------------------------------
+Same day delivery available in GTA аrea - delivery charges are extra depends upоn location
+------------------------------------------------------
+BUY NOW. PAY LATER.
+Get easy monthly financing when you shop with Canadian Outlet
+Split your purchase into stress-free, automatic installments with monthly Plans for -
+3 Months
+6 Months
+12 Months
+*All financing done through PayBright
+-------------------------------------------------------------------
+Storefront is open to public 7 days a week
+-------------------------------------------------------------------
+We are providing FREE parking facility for our customers (Contact us)!!
+-------------------------------------------------------------------
+STORE LOCATION:
+СANADIAN OUTLET
+1431 YONGE STREET
+YONGE &amp; ST CLAIR
+TORONTO, ON
+M4T 1Y7
+647 786 4344 (MAIN NUMBER)
+4164744786
+TIMINGS:
+MONDAY - FRIDAY: 8AM - 8PM
+WEEKENDS: 10AM - 7PM</t>
+  </si>
+  <si>
+    <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choiсe!
+Best Price, Best Quality
+Buy with Confidence from оur store! ✨
+------------------------------------------------------
+Samsung Phones - Samsung A35 5G, Samsung A34 5G, Samsung A33 5G, Samsung A31 phone
+BLOWOUT SALE!!!
+----------------------------------------------------------
+Samsung Galaxy A35 5G 128GB (Dual Sim)
+(Brand New In Box With Warranty)
+Price: $370 (Cash No Tax)
+----------------------------------------------------------
+Samsung Galaxy A34 5G 128GB (Dual Sim)
+(Brand New In Box With Warranty)
+Price: $335 (Cash No Tax)
+----------------------------------------------------------
+Samsung Galaxy A33 5G 128GB (Dual Sim)
+(Brand New In Box With Warranty)
+Price: $325 (Cash No Tax)
+----------------------------------------------------------
+Samsung Galaxy A31 64GB (Dual Sim)
+(Brand New In Box With Warranty)
+Price: $225 (Cash No Tax)
+----------------------------------------------------------
+Same day delivery available in GTА area-delivery charges are extra depends on location
+----------------------------------------------------------
+BUY NOW. PAY LATER.
+Get easy monthly financing when you shoр with Canadian Outlet
+Split your purchase into stress-free, automatic installments with monthly Plans for:-
+3 Mоnths
+6 Months
+12 Months
+*All financing done through Pаy Bright
+-------------------------------------------------------------------
+Storefront is open to public 7 days а week
+-------------------------------------------------------------------
+We are providing FREE parking facility for our customers (Contact us)!!
+-------------------------------------------------------------------
+STORE LOCATION:
+CANADIAN OUTLET
+1431 YONGE STREET
+YONGE &amp; ST CLAIR
+TОRONTO, ON
+M4T 1Y7
+647 786 4344 (MAIN NUMBER)
+4164744786
+TIMINGS:
+MONDAY - FRIDAY: 8AM - 8PM
+WEEKENDS: 10AM - 7PM</t>
+  </si>
+  <si>
+    <t>50-60</t>
+  </si>
+  <si>
+    <t>50-61</t>
+  </si>
+  <si>
+    <t>50-62</t>
+  </si>
+  <si>
+    <t>50-63</t>
+  </si>
+  <si>
+    <t>50-64</t>
+  </si>
+  <si>
+    <t>50-65</t>
+  </si>
+  <si>
+    <t>50-66</t>
+  </si>
+  <si>
+    <t>50-67</t>
+  </si>
+  <si>
+    <t>50-68</t>
+  </si>
+  <si>
+    <t>50-69</t>
+  </si>
+  <si>
+    <t>50-70</t>
+  </si>
+  <si>
+    <t>50-71</t>
+  </si>
+  <si>
+    <t>50-72</t>
+  </si>
+  <si>
+    <t>70-76</t>
+  </si>
+  <si>
+    <t>70-77</t>
+  </si>
+  <si>
+    <t>70-78</t>
+  </si>
+  <si>
+    <t>samsung</t>
+  </si>
+  <si>
+    <t>Macbook Air - 13 Inch, 8GB RAM, 256GB STORAGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
+Best Price, Best Quality 
+Buy with Confidence from our store! ✨
+------------------------------------------------------
+------------------------------------------------------
+BUY NOW. PAY LATER.
+Get easy monthly financing when you shop with Canadian Outlet
+Split your purchase into stress-free, automatic installments with monthly Plans for:-
+3 Months
+6 Months
+12 Months
+*All financing done through Pay Bright
+------------------------------------------------------
+Same day delivery available in GTA area - delivery charges are extra depends on location
+------------------------------------------------------
+Storefront is open to public 7 days a week
+------------------------------------------------------
+We are providing FREE parking facility for our customers (Contact us)!!
+------------------------------------------------------
+STORE LOCATION:
+CANADIAN OUTLET
+1431 YONGE STREET
+YONGE &amp; ST CLAIR
+TORONTO, ON
+M4T 1Y7
+647 786 4344 (MAIN NUMBER)
+416 474 4786
+TIMINGS:
+MONDAY - FRIDAY: 8AM - 8PM
+WEEKENDS: 10AM - 7PM
+</t>
+  </si>
+  <si>
+    <t>Macbook Air 8-256</t>
+  </si>
+  <si>
+    <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
+Best Price, Best Quality 
+Buy with Confidence from our store!
+------------------------------------------------------
+Dell Laptops Intel i5 - Dell inspiron 13, Dell 7480, Dell Latitude 7390, Dell Latitude 7420, Dell 5400, Dell Latitude 7400, Dell 7490, Dell 5490, Dell 3400, Dell 7480, Dell 5470 
+------------------------------------------------------
+Dell Latitude 7420 - 14" Touch
+INTEL i5 - 11th Generation
+16GB RAM
+256GB SSD
+(LIKE NEW IN BOX WITH WARRANTY)
+PRICE - $545 (CASH NO TAX)
+------------------------------------------------------
+Dell inspiron 13
+Intel i5 - 8th Generation
+16GB RAM
+512GB SSD
+(LIKE NEW IN BOX WITH WARRANTY)
+PRICE - $425 (CASH NO TAX)
+------------------------------------------------------
+Dell 7480 - 14" Touch
+Intel i5 - 7th Generation
+16GB RAM
+512GB SSD
+(LIKE NEW IN BOX WITH WARRANTY)
+PRICE - $395 (CASH NO TAX)
+------------------------------------------------------
+Dell 7410 
+INTEL i5 - 10th Generation
+16GB RAM
+512GB SSD
+(LIKE NEW IN BOX WITH WARRANTY)
+PRICE - $375 (CASH NO TAX)
+------------------------------------------------------
+Dell Latitude 7390 (Touchscreen) - 13.3"
+INTEL i5 - 8th Generation
+16GB RAM
+512GB SSD
+(LIKE NEW IN BOX WITH WARRANTY)
+PRICE - $325 (CASH NO TAX) 
+------------------------------------------------------
+Dell 5400 - 14"
+Intel i5 - 8th Generation
+16GB RAM
+256GB SSD
+(LIKE NEW IN BOX WITH WARRANTY)
+PRICE - $295 (CASH NO TAX) 
+------------------------------------------------------
+Dell Latitude 7400 - 14" Webcam
+INTEL i5 - 8th Generation
+16GB RAM
+256GB SSD
+(LIKE NEW IN BOX WITH WARRANTY)
+PRICE - $275 (CASH NO TAX)
+------------------------------------------------------
+Dell 5490 (Touchscreen)- 14"
+Intel i5 - 8th Generation
+8GB RAM
+256GB SSD
+(LIKE NEW IN BOX WITH WARRANTY)
+PRICE - $275 (CASH NO TAX)
+-----------------------------------------
+Dell 3400 - 14" Webcam
+Intel i5 - 8th Generation
+8GB RAM
+256GB SSD
+(LIKE NEW IN BOX WITH WARRANTY)
+PRICE - $250(CASH NO TAX)
+-----------------------------------------
+Dell 7490 - 14"
+Intel i5 - 8th Generation
+8GB RAM
+256GB SSD
+(LIKE NEW IN BOX WITH WARRANTY)
+PRICE - $245 (CASH NO TAX)
+Dell 7490 - 14"
+Intel i5 - 7th Generation
+16GB RAM
+256GB SSD
+(LIKE NEW IN BOX WITH WARRANTY)
+PRICE - $225 (CASH NO TAX) 
+-----------------------------------------
+Dell 7480 - 14"
+Intel i5 - 7th Generation
+16GB RAM
+256GB SSD
+(LIKE NEW IN BOX WITH WARRANTY)
+PRICE - $225 (CASH NO TAX)
+-----------------------------------------
+Dell 7480 - 14"
+Intel i5 - 6th Generation
+8GB RAM
+256GB SSD
+(LIKE NEW IN BOX WITH WARRANTY)
+PRICE - $195 (CASH NO TAX) (SOLD OUT)
+-----------------------------------------
+Dell 5470 14"
+Intel i5 - 6th Generation
+8GB RAM
+256GB SSD
+(LIKE NEW IN BOX WITH WARRANTY)
+PRICE - $195(CASH NO TAX) (SOLD OUT)
+-----------------------------------------
+Same day delivery available in GTA area -delivery charges are extra depends on location
+-----------------------------------------
+BUY NOW. PAY LATER.
+Get easy monthly financing when you shop with Canadian Outlet
+Split your purchase into stress-free, automatic installments with monthly Plans for:-
+3 Months
+6 Months
+12 Months
+*All financing done through Pay Bright
+-------------------------------------------------------------------
+Storefront is open to public 7 days a week
+-------------------------------------------------------------------
+We are providing FREE parking facility for our customers (Contact us)!!
+-------------------------------------------------------------------
+STORE LOCATION:
+CANADIAN OUTLET
+1431 YONGE STREET
+YONGE &amp; ST CLAIR
+TORONTO, ON
+M4T 1Y7
+647 786 4344 (MAIN NUMBER)
+416 474 4786
+TIMINGS:
+MONDAY - FRIDAY: 8AM - 8PM
+WEEKENDS: 10AM - 7PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apple iPhone 15 128GB BRAND NEW </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
+Best Price, Best Quality 
+Buy with Confidence from our store! ✨
+------------------------------------------------------
+Apple iPhone 15 128GB
+(BRAND NEW WITH APPLE WARRANTY)
+PRICE - $975 (CASH NO TAX)
+------------------------------------------------------
+BUY NOW. PAY LATER.
+Get easy monthly financing when you shop with Canadian Outlet
+Split your purchase into stress-free, automatic installments with monthly Plans for:-
+3 Months
+6 Months
+12 Months
+*All financing done through Pay Bright
+------------------------------------------------------
+Same day delivery available in GTA area - delivery charges are extra depends on location
+------------------------------------------------------
+Storefront is open to public 7 days a week
+------------------------------------------------------
+We are providing FREE parking facility for our customers (Contact us)!!
+------------------------------------------------------
+STORE LOCATION:
+CANADIAN OUTLET
+1431 YONGE STREET
+YONGE &amp; ST CLAIR
+TORONTO, ON
+M4T 1Y7
+647 786 4344 (MAIN NUMBER)
+416 474 4786
+TIMINGS:
+MONDAY - FRIDAY: 8AM - 8PM
+WEEKENDS: 10AM - 7PM
+</t>
+  </si>
+  <si>
+    <t>iPhone 15</t>
+  </si>
+  <si>
+    <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
+Best Price, Best Quality
+Buy with Confidence from our store!
+------------------------------------------------------
+Samsung Phones - A15, A14, A13, A12, A11, A10S, A10E
+------------------------------------------------------
+Samsung Galaxy A15 5G 128GB/ 6GB (Dual SIM)
+(Brand New In Box With Warranty)
+Price - $210 (Cash No Tax)
+Samsung Galaxy A15 5G 128GB (Dual SIM)
+(Like New In Box With Warranty)
+Price - $180 (Cash No Tax)
+------------------------------------------------------
+Samsung Galaxy A15 128GB (Dual SIM)
+(Brand New In Box With Warranty)
+Price - $165 (Cash No Tax)
+------------------------------------------------------
+Samsung Galaxy A14 128GB (Dual SIM)
+(New In Box With Warranty)
+Price - $165 (Cash No Tax)
+Samsung Galaxy A14 64GB (Dual SIM)
+(New In Box With Warranty)
+Price - $155 (Cash No Tax)
+Samsung Galaxy A14 5G 64GB
+(New Open Box With 6 Months Store Warranty)
+Price - $165 (Cash No Tax)
+---------------------------------------------------
+Samsung Galaxy A13 4GB/128GB (Dual Sim)
+(New in Box with Warranty)
+Price: $175 (Cash No Tax)
+Samsung Galaxy A13 4GB/64GB (Dual Sim)
+(New in Box with Warranty)
+Рrice: $160 (Cash No Tax)
+Samsung Galaxy A13 5G 4GB/64GB
+(Like New in Box with Warranty)
+Price: $135 (Cash No Tax)
+------------------------------------------------------
+Samsung Galaxy A12 128GB (Dual Sim)
+(New Open Box With Warranty)
+Price: $165 (Cash No Tax)
+Samsung Galaxy A12 64GB/ 4GB RAM (Dual Sim)
+(New In Box With Warranty)
+Price: $145 (Cash No Tax)
+Samsung Galaxy A12 32GB
+(Like New In Box With Warranty)
+Price: $135 (Cash No Tax)
+------------------------------------------------------
+Samsung Galaxy A11 32GB
+(New In Box With Warranty)
+Price: $125 (Cash No Tax)
+Samsung Galaxy A11 32GB
+(Fully Functional with Warranty)
+Price: $110 (Cash No Tax)
+------------------------------------------------------
+Samsung Galaxy A10s 32GB (Dual Sim)
+(Like Nеw In Box With Warranty)
+Price: $105 (Cash No Tax)
+------------------------------------------------------
+Samsung Galaxy A10E 32GB
+(Fully Functional with Warranty)
+Price: $95 (Cash No Tax)
+------------------------------------------------------
+Same day delivery available in GTA area - delivery charges are extra depends on location
+---------------------------------------------------
+BUY NOW. PAY LATER.
+Get easy mоnthly financing when you shop with Canadian Outlеt
+Split your purchase into stress-free, automаtic installments with monthly Plans for:-
+3 Mоnths
+6 Months
+12 Months
+*All financing done through Pay Bright
+---------------------------------------------------
+Storefront is open to рublic 7 days a week
+----------------------------------------------------
+We are providing a FREЕ parking facility for our customers (Contact us)!!
+----------------------------------------------------
+STORE LOCATION:
+CANADIAN OUTLET
+1431 YONGE STREET
+YONGE &amp; ST CLAIR
+TORONTO, ON
+M4T 1Y7
+647 786 4344 (MAIN NUMBER)
+416 474 4786
+TIMINGS:
+MONDAY - FRIDAY: 8AM - 8PM
+WEEKENDS: 10AM - 7PM</t>
+  </si>
+  <si>
+    <t>Shop Smart, Shop Secure: Canadian Outlеt, Your Trusted Choice!
+Best Price, Best Quality
+Buy with Confidence from our store!
+------------------------------------------------------
+LG Phones - LG G7 ThinQ, LG V60 ThinQ, LG G8 ThinQ, LG V40, LG V30, LG Velvet 5G, LG Phoenix 5, K50s, V20
+BLOWOUT SALE!!!
+------------------------------------------
+LG V60 ThinQ 128GB Unlocked
+(Like New in Box with warranty)
+Price - $275 (Cash No Tax)
+------------------------------------------
+LG Velvet 5G 128GB Unlocked
+(Open Box with warranty)
+Price - $225 (Cash No Tax)
+------------------------------------------
+LG G8 ThinQ 128GB Unlocked
+(Brand New in Box with warranty)
+Price - $245 (Cash No Tax)
+LG G8 ThinQ 128GB Unlocked
+(Like New in Box with warranty)
+Price - $195 (Cash No Tax)
+------------------------------------------
+LG Stylo 6 64GB Unlocked
+(Brand new in box with warranty)
+Price - $195 (Cash No Tax)
+LG Stylo 6 64GB Unlocked
+(Like new in box with warranty)
+Price - $145 (Cash No Tax)
+-------------------------------------------
+LG V40 ThinQ 64GB Unlocked
+(Like New in Box with warranty)
+Price - $175 (Cash No Tax)
+------------------------------------------
+LG V30 64GB Unlocked
+(Brand new in box with warranty)
+Price - $175 (Cash No Tax)
+------------------------------------------
+LG G7 ThinQ 64GB Unlocked
+(Like New in Box with warranty)
+Price - $165 (Cash No Tax)
+------------------------------------------
+LG V20 64GB Unlocked Smartphone
+(Like New in Box with Warranty)
+Price - $145 (Сash No Tax)
+--------------------------------------------
+LG K50s 32GB Unlocked
+(Brand new in box with warranty)
+Price - $160 (Cash No Tax)
+-------------------------------------------
+LG Pheonix 5 16GB Unlocked
+(Like New in Box with warranty)
+Price - $95 (Cash No Tax)
+-------------------------------------------
+Same day delivery available in GTA area - delivery charges are extra depends on location
+----------------------------------------------------
+BUY NOW. PAY LATER.
+Get easy monthly financing when you shop with Canadian Outlet
+Split yоur purchase into stress-free, automatic installments with monthly Plans for:-
+3 Months
+6 Months
+12 Months
+*All financing done through Pay Bright
+-------------------------------------------------------------------
+Stоrefront is open to public 7 days a week
+-------------------------------------------------------------------
+We are providing FREE parking facility for our customers (Contact us)!!
+-------------------------------------------------------------------
+STORE LOCATION:
+CANADIAN OUTLET
+1431 YONGE STREET
+YONGE &amp; ST CLAIR
+TORONTO, ON
+M4T 1Y7
+647 786 4344 (MAIN NUMBER)
+416 474 4786
+TIMINGS:
+MONDAY - FRIDAY: 8AM - 8PM
+WEEKENDS: 10AM - 7PM</t>
+  </si>
+  <si>
+    <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
+Best Price, Best Quality
+Buy with Confidеnce from our store!
+------------------------------------------------------
+HP Laptops Intel i5 - HP EliteBook 840 G9, HP PrоBook 440 G3, HP ELITEBOOK 840 G7, HР ELITEBOOK 840 G6, HP Probook 430 G5, HP 15 DY2795WM, HP ProBook 430 G3, HP ELITEBOOK 840 G4, HP ELITEBOOK 840 G6, HP EliteBook Folio 9470M
+------------------------------------------------------
+HP EliteBook 840 G9 - 14"
+Intel Core i5 - 12th Gen
+16GB RAM
+512GB SSD
+Intel Iris XЕ Graphics
+Windows 11 Pro
+(BRAND NЕW IN BOX WITH WARRANTY)
+PRICE - $1295 (CASH NO TAX)
+------------------------------------------------------
+HP 15 DY2795WM 15.6
+INTEL i5 - 11TH GEN
+8GB RAM
+256GB SSD
+(Brand New In Box With Warranty)
+PRICE - $595 (CASH NO TAX)
+------------------------------------------------------
+HP ELITEBOOK 840 G7 - 14"
+INTEL i5 - 10TH GEN
+16GB RAM
+256GB SSD
+(LIKE NEW IN BOX WITH WARRANTY)
+PRICE - $475 (CASH NO TAX)
+------------------------------------------------------
+HP ELITEBOOK 840 G6 - 14"
+INTEL i5 - 8TH GEN
+16GB RAM
+256GB SSD
+(LIKE NEW IN BOX WITH WARRANTY)
+PRICE - $325(CASH NO TAX)
+-----------------------------------------------------
+HP ProBook 430 G3 13.3" (Touchscrеen)
+INTEL i5 - 6TH GEN
+8GB RAM
+256GB SSD
+(LIKE NEW IN BOX WITH WARRАNTY)
+PRICE - $325 (CASH NO TAX)
+------------------------------------------------------
+HP ELITEBOOK 840 G6 - 14"
+INTEL i5 - 8TH GEN
+8GB RAM
+256GB SSD
+(LIKE NEW IN BОX WITH WARRANTY)
+PRICE - $295(CASH NO TAX)
+------------------------------------------------------
+HP Probook 430 G5 - 13.3"
+INTEL i5 - 8TH GEN
+16GB RAM
+256GB SSD
+(LIKE NEW IN BOX WITH WARRANTY)
+PRIСE - $275(CASH NO TAX)
+------------------------------------------------------
+Same day delivery availablе in GTA area -delivery charges are еxtra depends on location
+------------------------------------------------------
+BUY NOW. PAY LATER.
+Get easy monthly financing when you shоp with Canadian Outlet
+Split your purchase into stress-free, automatic installments with monthly Plans fоr:-
+3 Months
+6 Months
+12 Months
+*All financing done through Pay Bright
+------------------------------------------------------
+Storefront is open to public 7 days a week
+------------------------------------------------------
+We are providing FREE parking facility for our customers (Contact us)!!
+------------------------------------------------------
+STORE LOCATION:
+CANADIAN OUTLET
+1431 YONGE STREET
+YONGE &amp; ST CLAIR
+TORONTO, ON
+M4T 1Y7
+647 786 4344 (MAIN NUMBER)
+4164744786
+TIMINGS:
+MONDAY - FRIDAY: 8AM - 8PM
+WEEKENDS: 10AM - 7PM</t>
+  </si>
+  <si>
+    <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
+Best Price, Best Quality
+Buy with Confidence from our store! ✨
+---------------------------------------------
+Samsung Phones - Samsung Galaxy A05s, Samsung Galaxy A05, Samsung Galaxy A04, Samsung Galaxy A04e, Samsung Galaxy A03s, Samsung Galaxy A02s, Samsung Galaxy A02, Samsung Galaxy A03 Core phone
+Samsung Galaxy A05s 128GB (Dual Sim)
+(New In Box With Warranty)
+Price: $175 (Cash No Tax)
+Samsung Galaxy A05s 64GB (Dual Sim)
+(New In Box With Warranty)
+Price: $150 (Cash Nо Tax)
+Samsung Galaxy A05 128GB (Dual Sim)
+(New In Box With Warranty)
+Price: $140 (Cash No Tax)
+Samsung Galaxy A05 64GB (Dual Sim)
+(New In Box With Warranty)
+Priсe: $135 (Cash No Tax)
+---------------------------------------------
+Samsung Galaxy A04 64GB (Dual Sim)
+(New In Box With Warranty)
+Price: $135 (Cash No Tax)
+Samsung Galaxy A04 32GB (Dual Sim)
+(Nеw In Box With Warranty)
+Price: $115 (Cash No Tax)
+---------------------------------------------
+Sаmsung Galaxy A04e 64GB (Dual Sim)
+(New In Box With Warranty)
+Pricе: $125 (Cash No Tax)
+Samsung Galaxy A04e 32GB (Dual Sim)
+(New In Box With Warranty)
+Price: $105 (Cash No Tax)
+---------------------------------------------
+Sаmsung Galaxy A03s 32GB
+(New In Bоx With Warranty)
+Price: $125 (Cаsh No Tax)
+---------------------------------------------
+Samsung Galaxy A02s 32GB (Dual Sim)
+(New In Box With Warranty)
+Price: $125 (Cash No Tax)
+---------------------------------------------
+Sаmsung Galaxy A02 32GB (Dual Sim)
+(New In Box With Warranty)
+Price: $115 (Cash No Tax)
+---------------------------------------------
+Samsung Galaxy A03 Core 32GB
+(New In Box With Warranty)
+Priсe: $100 (Cash No Tax)
+---------------------------------------------
+Same day delivery available in GTA area -delivery charges are extra depends on location
+---------------------------------------------
+BUY NOW. PAY LATER.
+Get easy monthly financing when you shop with Сanadian Outlet
+Split your purchasе into stress-free, automatic installments with monthly Plans for:-
+3 Months
+6 Months
+12 Months
+*Аll financing done through Pay Bright
+-------------------------------------------------------------------
+Storefront is open to public 7 days a week
+-------------------------------------------------------------------
+We are providing FREE рarking facility for our customers (Contact us)!!
+-------------------------------------------------------------------
+STORE LOCATION:
+CANADIAN OUTLET
+1431 YONGE STREET
+YONGE &amp; ST CLAIR
+TORONTO, ON
+M4T 1Y7
+647 786 4344 (MAIN NUMBER)
+4164744786
+TIMINGS:
+MONDAY - FRIDAY: 8AM - 8PM
+WEEKENDS: 10AM - 7PM</t>
+  </si>
+  <si>
+    <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
+Best Price, Best Quality
+Buy with Confidence from our storе!
+---------------------------------------------
+Samsung Phones - Samsung A25, Samsung A24, Samsung A23, Samsung A22, Samsung A21S
+BLOWOUT SALE!!!
+---------------------------------------------
+Samsung Galaxy A25 5G 128GB (Dual Sim)
+(Brand New In Box With Warranty)
+Priсe: $250 (Cash No Tax)
+---------------------------------------------------
+Samsung Galaxy А24 128GB (Dual Sim)
+(Brand Nеw In Box With Warranty)
+Pricе: $235 (Cash No Tax)
+---------------------------------------------------
+Samsung Galaxy A23 128GB (Dual Sim)
+(Brand New In Box With Warranty)
+Price: $215 (Cash No Tax)
+Samsung Galaxy A23 64GB (Dual Sim)
+(Brand New In Box With Warranty)
+Price: $200 (Cash No Tax)
+---------------------------------------------
+Samsung Galaxy A22 128GB (Dual Sim)
+(Brand New In Box With Warranty)
+Price: $210 (Cash No Tax)
+Samsung Galaxy A22 64GB (Dual Sim)
+(Brand New In Box With Warranty)
+Price: $200 (Cash No Tax)
+Samsung Galaxy A22 5G 64GB (Dual Sim)
+(Brand New In Box With Warranty)
+Price: $210 (Cаsh No Tax)
+---------------------------------------------
+Samsung Galaxy A21S 128GB (Dual Sim)
+(Brand New In Box With Wаrranty)
+Price: $200 (Cash No Tax)
+Samsung Galaxy A21S 64GB (Dual Sim)
+(Brand New In Box With Warranty)
+Price: $190 (Cash No Tax)
+---------------------------------------------
+Same day delivery availablе in GTA area - delivery charges are extra depends on location
+---------------------------------------------------
+BUY NOW. PAY LATER.
+Get easy monthly finаncing when you shop with Canadiаn Outlet
+Split your purchase into stress-free, automatic installments with monthly Plans for:-
+3 Months
+6 Months
+12 Months
+*All financing done through Pay Bright
+-------------------------------------------------------------------
+Storefront is open to public 7 days a week
+-------------------------------------------------------------------
+We are providing FREE parking facility for our customers (Contact us)!!
+-------------------------------------------------------------------
+STORE LOCАTION:
+CANADIAN OUTLET
+1431 YONGE STREET
+YONGE &amp; ST CLAIR
+TORONTO, ON
+M4T 1Y7
+647 786 4344 (MAIN NUMBER)
+4164744786
+TIMINGS:
+MONDAY - FRIDAY: 8AM - 8PM
+WEEKENDS: 10AM - 7PM</t>
+  </si>
+  <si>
+    <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
+Best Price, Best Quality
+Buy with Cоnfidence from our store!
+---------------------------------------------
+BLOWOUT SALE!!!
+Samsung Gаlaxy S24 Ultra, Samsung Galaxy S24, Samsung Galaxy S23 Ultra, Samsung Galaxy S23, Samsung Galaxy S23+, Sаmsung Galaxy S23 FE, Samsung Galaxy S22 Ultra, Samsung Galaxy S22+, Sаmsung Galaxy S22
+-----------------------------------------------------------------------
+Samsung Galаxy S24 Ultra 12GB / 512GB (DUAL SIM)
+(Brand New in Box with 1 Year Warranty)
+Price - $1545 (CASH NО TAX)
+Samsung Galaxy S24 Ultrа 12GB / 256GB (CANADIAN MODEL)
+(Brand New Open Box with Warranty)
+Price - $1095 (CASH NO TAX)
+-----------------------------------------------------------------------
+Samsung Galaxy S24 256GB (CANADIAN MODEL)
+(Brand New in Box with 1 Year Samsung Warranty)
+PRICE - $825 (CASH NO TAX)
+Samsung Galaxy S24 256GB (CANADIAN MODEL)
+(Like New in Box with Warranty)
+PRICE - $750 (CASH NO TAX)
+Samsung Galaxy S24 128GB (CANADIAN MODEL)
+(Brand New in Box with 1 Year Samsung Warranty)
+PRICE - $740 (CASH NO TAX)
+Samsung Galaxy S24 128GB (CANADIAN MODEL)
+(Like New in Box with Warranty)
+PRICE - $695 (CASH NO TAX)
+-----------------------------------------------------------------------
+Samsung Galaxy S23 Ultra 512GB (DUAL SIM)
+(Brand New in Box with 1 Year Warranty)
+Price - $1250 (CASH NO TAX)
+Samsung Galaxy S23 Ultra 512GB
+(Like New in Box with Warranty)
+Price - $995 (CASH NO TAX)
+Samsung Galaxy S23 Ultra 256GB (DUAL SIM)
+(Brаnd New in Box with 1 Year Warranty)
+Price - $1095 (CASH NO TAX)
+Samsung Galaxy S23 Ultra 256GB
+(Like New in Box with Warranty)
+Price - $950 (CASH NO TAX)
+---------------------------------------------
+Samsung Galaxy S23+ 256GB (DUAL SIM)
+(Brand New in Box with 1 Year Warranty)
+Price - $945 (CASH NO TAX)
+---------------------------------------------
+Samsung Galaxy S23 256GB (CANADIAN MODEL)
+(Brand New Open Box with Samsung Warranty)
+Price - $795 (CASH NO TAX)
+Samsung Galaxy S23 128GB (CANADIAN MODEL)
+(Brand New in Box with 1 Year Samsung Warranty)
+Price - $735 (CASH NO TAX)
+Samsung Galaxy S23 5G 128GB
+(New Open Box with 6 Months Warranty)
+Price - $625 (CASH NO TAX)
+---------------------------------------------
+Samsung Galaxy S23 FE 5G 256GB (DUAL SIM)
+(Brand New in Box with 1 Year Warranty)
+Price - $645 (CASH NO TAX)
+Samsung Galaxy S23 FE 5G 256GB
+(Like New in Box with Warranty)
+Price - $575 (CАSH NO TAX)
+Samsung Galaxy S23 FЕ 5G 128GB (CANADIAN MODEL)
+(Brand New in Box with 1 Year Samsung Warranty)
+Price - $595 (CASH NO TAX)
+Samsung Galaxy S23 FE 5G 128GB
+(Like New in Box with Warranty)
+Рrice - $500 (CASH NO TAX)
+---------------------------------------------
+Samsung Galaxy S22 Ultra 5G 512GB
+(LIKE NEW IN BOX WITH WARRANTY)
+PRICE: $695 (CASH NO TAX)
+Samsung Galaxy S22 Ultra 5G 256GB
+(LIKE NEW IN BOX WITH WARRANTY)
+PRICE: $645 (CASH NO TAX)
+Samsung Galaxy S22 Ultra 5G 128GB
+(LIKE NEW IN BOX WITH WARRANTY)
+PRICE: $595 (CASH NO TAX)
+---------------------------------------------
+Sаmsung Galaxy S22+ (Plus) 5G 256GB
+(LIKE NEW IN BOX WITH WARRANTY)
+PRICE: $495 (CASH NO TAX)
+Samsung Galaxy S22+ (Plus) 5G 128GB
+(LIKE NEW IN BOX WITH WARRANTY)
+PRICE: $445 (CASH NO TAX)
+---------------------------------------------
+Samsung Galaxy S22 5G 256GB
+(LIKE NEW IN BOX WITH WARRANTY)
+PRICЕ: $395 (CASH NO TAX)
+Samsung Galaxy S22 5G 128GB
+(LIKE NEW IN BOX WITH WARRANTY)
+PRICE: $375 (CASH NO TAX)
+---------------------------------------------
+Same day dеlivery available in GTA area - delivery charges are extra depends on location
+------------------------------------------------------------------------
+BUY NOW. PAY LATER.
+Get easy monthly financing when you shop with Canadian Outlet
+Sрlit your purchase into stress-free, automatic installments with monthly Plans for:-
+3 Months
+6 Months
+12 Months
+*All financing done through Pay Bright
+---------------------------------------------
+Storefront is open to public 7 days a week
+---------------------------------------------
+We are providing FREE parking facility for our customers (Contact us)!!
+---------------------------------------------
+STORE LOCATION:
+CANADIAN OUTLЕT
+1431 YONGE STREET
+YONGE &amp; ST CLAIR
+TORONTO, ON
+M4T 1Y7
+647 786 4344 (MAIN NUMBER)
+416 474 4786
+TIMINGS:
+MONDAY - FRIDAY: 8AM - 8PM
+WEEKENDS: 10AM - 7PM</t>
+  </si>
+  <si>
+    <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
+Best Price, Best Quality
+Buy with Confidence from our store! ✨
+---------------------------------------------
+JBL Harman Endurance Race, JBL Vibe Beam In-Ear Sound Isolating Truly Wireless Headphones, JBL Run 2, JBL 215 BT, JBL 125BT
+---------------------------------------------------
+JBL Vibe Beam In-Ear Sound Isolating Truly Wireless Headphones
+(BRAND NEW IN BOX)
+PRICE - $70 (CASH NO TAX)                                                                                                                                                                                                                                                                                                                   
+                                                                                                                                                                                                                                                                                                                                                                                                                                            JBL Harman Endurance Race Waterproof True Wireless Active Sport Earbuds
+(BRAND NEW IN BOX)
+Price - $60 (CASH NO TAX)
+JBL Еndurance RUN 2 In-Ear Wireless Sport Headphones
+(BRAND NEW IN BOX)
+Price - $35 (CASH NO TAX)
+JBL Tune 215BT Wireless Earbud headphones
+(BRAND NEW IN BOX)
+Price - $35 (CASH NO TAX)
+JBL Tune 125BT Wireless Earbud headphones
+(BRAND NEW IN BOX)
+Price - $35 (CASH NO TAX)
+---------------------------------------------------
+Same day dеlivery available in GTA area - delivery charges are extra depends on location
+---------------------------------------------------
+BUY NOW. PAY LATER.
+Get easy monthly financing when you shop with Canadian Outlet
+Split your purchase into stress-free, automatic installments with monthly Plans for:-
+3 Months
+6 Months
+12 Months
+*All financing done through Pay Bright
+-------------------------------------------------------------------
+Storefront is open to public 7 days a week
+-------------------------------------------------------------------
+We are providing a FREE parking facility for our customers (Contact us)!!
+-------------------------------------------------------------------
+STORE LOCATION:
+CANADIAN OUTLET
+1431 YONGE STREET
+YONGE &amp; ST CLAIR
+TORONTO, ON
+M4T 1Y7
+647 786 4344 (MAIN NUMBER)
+416 474 4786
+TIMINGS:
+MONDAY - FRIDAY: 8AM - 8PM
+WEEKENDS: 10АM - 7PM</t>
+  </si>
+  <si>
+    <t>ASTRO Gaming A50 Wireless Headset + Base Station</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
+Best Price, Best Quality 
+Buy with Confidence from our store! ✨
+------------------------------------------------------
+ASTRO Gaming A50 Wireless Headset + Base Station Gen 4 - Compatible With PS5, PS4, PC, Mac
+(Brand New in Box)
+Price - $260 (Cash No Tax)
+ASTRO Gaming A50 Wireless + Base Station for Xbox One and Series X &amp; PC
+(Brand New in Box)
+Price - $260 (Cash No Tax)
+------------------------------------------------------
+BUY NOW. PAY LATER.
+Get easy monthly financing when you shop with Canadian Outlet
+Split your purchase into stress-free, automatic installments with monthly Plans for:-
+3 Months
+6 Months
+12 Months
+*All financing done through Pay Bright
+------------------------------------------------------
+Same day delivery available in GTA area - delivery charges are extra depends on location
+------------------------------------------------------
+Storefront is open to public 7 days a week
+------------------------------------------------------
+We are providing FREE parking facility for our customers (Contact us)!!
+------------------------------------------------------
+STORE LOCATION:
+CANADIAN OUTLET
+1431 YONGE STREET
+YONGE &amp; ST CLAIR
+TORONTO, ON
+M4T 1Y7
+647 786 4344 (MAIN NUMBER)
+416 474 4786
+TIMINGS:
+MONDAY - FRIDAY: 8AM - 8PM
+WEEKENDS: 10AM - 7PM
+</t>
+  </si>
+  <si>
+    <t>Astro Gaming</t>
+  </si>
+  <si>
+    <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
+Best Price, Best Quality
+Buy with Confidence from our store! ✨
+---------------------------------------------
+Samsung Galaxy Buds2 Pro Headphones, Samsung Galaxy Buds2 Headphones, Samsung Galaxy Buds FE, Samsung Galaxy Buds Headрhones
+---------------------------------------------------
+Samsung Galaxy Buds2 Pro In-Ear Noise Сancelling Truly Wireless Headphones
+(BRAND NEW IN BOX WITH WARRANTY)
+PRICE - $145 (CASH NO TAX)
+Samsung Galaxy Buds2 In-Ear Noise Cancelling Truly Wireless Headphones
+(BRAND NEW IN BOX WITH WARRANTY)
+PRICE - $75 (CASH NO TAX)
+Samsung Galaxy Buds FE Truly Wireless Bluetooth Earbuds, Active Noise Cancellation(ANC)
+(BRAND NEW IN BOX WITH WARRANTY)
+PRICE - $85 (CASH NO TAX)
+---------------------------------------------------
+Same day delivery available in GTA area - delivery charges are extra depends on loсation
+---------------------------------------------------
+BUY NОW. PAY LATER.
+Get easy monthly financing when you shop with Canadian Outlet
+Split your purchаse into stress-free, automatic installments with monthly Plans for:-
+3 Months
+6 Months
+12 Months
+*All financing done through Pay Bright
+---------------------------------------------------
+Storefront is open to public 7 days a week
+----------------------------------------------------
+We are providing a FREE parking facility for our customers (Contаct us)!!
+----------------------------------------------------
+STORE LOCATION:
+CANADIAN OUTLЕT
+1431 YONGE STREET
+YONGE &amp; ST CLAIR
+TORONTO, ON
+M4T 1Y7
+647 786 4344 (MAIN NUMBER)
+416 474 4786
+TIMINGS:
+MONDAY - FRIDАY: 8AM - 8PM
+WEEKENDS: 10AM - 7РM</t>
+  </si>
+  <si>
+    <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
+Best Price, Best Quality
+Buy with Confidence from our store! ✨
+---------------------------------------------
+Bose QuietComfort Ultra Headphones, QuietComfort and QuietComfort 45 Bluetooth Headphones, Bose Ultra Earbuds
+---------------------------------------------------
+Bose QuietComfort Ultra Wireless Noise Cancelling Headрhones
+(BRAND NEW IN BOX WITH 1 YEAR MANUFACTURER WARRANTY)
+PRICE - $445 (CASH NO TAX)
+---------------------------------------------------
+Bose QuietComfort Wireless Noise Cancelling Headphones
+(BRAND NEW IN BOX WITH 1 YEAR MANUFACTURER WARRANTY)
+PRICE - $375 (CASH NO TAX)
+Bose QuietComfort 45 Over-Ear Noise Cancelling Bluetooth Headphоnes
+(BRAND NEW IN BOX WITH 1 YEAR MANUFACTURER WАRRANTY)
+PRICE - $345(CASH NO TAX)
+---------------------------------------------------
+Bose QuiеtComfort Ultra Wireless Noise Cancelling Earbuds, Bluetooth Noise Cancelling Earbuds with Spatial Audio and World-Class Noise Cancellation
+(BRAND NEW IN BOX WITH WARRANTY)
+PRICE - $275 (CASH NO TAX)
+---------------------------------------------------
+Bose QuietComfort Ultra Wireless Noise Cancelling Earbuds, Bluetooth Noise Cancelling Earbuds with Spatial Audio and World-Class Noise Canсellation
+(NEW OPEN BOX WITH WARRANTY)
+PRICE - $225 (CASH NO TAX)
+---------------------------------------------------
+Same day delivery availаble in GTA area - delivery charges are extra depends on location
+---------------------------------------------------
+BUY NOW. PAY LATER.
+Get easy monthly financing when you shop with Canadian Outlet
+Split your purchase into stress-free, automatic installments with monthly Plans for:-
+3 Mоnths
+6 Months
+12 Months
+*All financing done through Pay Bright
+-------------------------------------------------------------------
+Storefront is open to public 7 days a week
+-------------------------------------------------------------------
+We are providing FREE parking facility for our customers (Contact us)!!
+-------------------------------------------------------------------
+STORE LOCATION:
+CANADIAN OUTLET
+1431 YONGE STREET
+YОNGE &amp; ST CLAIR
+TORONTO, ON
+M4T 1Y7
+647 786 4344 (MAIN NUMBER)
+4164744786
+TIMINGS:
+MONDAY - FRIDAY: 8AM - 8PM
+WEEKENDS: 10AM - 7PM</t>
+  </si>
+  <si>
+    <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choiсe!
+Best Price, Best Quality
+Buy with Confidence from оur store! ✨
+---------------------------------------------------
+Beats Studio Pro, Beats Studio3 Headphones, Powеrbeats Pro Headphones, Beats By Dr. Dre Fit Pro, Beats Studio Buds + Earbuds, Beats Studio Buds, Powerbeats 3
+---------------------------------------------------
+Beats Studio Pro - Wireless Bluetooth Noise Cancelling Headphones
+(BRAND NEW IN BOX)
+Price - $295 (Cash No Tax)
+Beats Beаts Studio3 Wireless Over-Ear Headphones
+(BRAND NEW IN BOX)
+Price - $225 (Cash No Tax)
+---------------------------------------------------
+Beats Powerbeats Pro In-Ear Truly Wireless Headphones
+(BRAND NEW IN BOX)
+PRICE - $195 (CASH NO TAX)
+------------------------------------------------------
+Beats Powerbeats Pro In-Ear Truly Wireless Headphones
+(LIKE NEW IN BOX)
+PRICE - $145 (CASH NO TАX)
+------------------------------------------------------
+Beats Fit Pro X Alo Special Edition In-Ear Noise Cancеlling True Wireless Earbuds (BRAND NEW IN BOX)
+PRICE - $195 (CASH NO TAX)
+Beats Fit Pro In-Ear Noise Cancelling True Wireless Earbuds
+(BRAND NEW IN BOX)
+PRICE - $175 (CASH NO TAX)
+------------------------------------------------------
+Beats Studio Budsplus [+] True Wireless Noise Cancelling Earbuds
+(BRAND NEW IN BOX)
+PRICE - $145 (СASH NO TAX)
+------------------------------------------------------
+Beats Studio Buds In-Ear Noise Cancelling True Wireless Earbuds
+(BRAND NEW IN BOX)
+PRICE - $115 (CASH NO TAX)
+------------------------------------------------------
+Beats Studio Buds In-Ear Noise Cancelling True Wireless Earbuds
+(LIKE NEW IN BOX)
+PRICE - $85 (CASH NO TAX)
+------------------------------------------------------
+Beats Powerbeats3 Wireless in-Ear Headphones - White
+(BRAND NEW IN BOX)
+PRICE - $65 (CASH NO TAX)
+------------------------------------------------------
+Samе day delivery available in GTA area - delivery charges are extra depends on location
+------------------------------------------------------
+BUY NOW. PAY LATER.
+Get easy monthly financing when you shop with Canadian Outlet
+Split your purchase into stress-free, automatic installments with monthly Plans for:-
+3 Months
+6 Months
+12 Months
+*Аll financing done through Pay Bright
+---------------------------------------------------
+Storefront is open to public 7 days a week
+----------------------------------------------------
+We are providing a FREE parking facility for our customers (Contact us)!!
+----------------------------------------------------
+STORE LOCATION:
+CANADIAN OUTLET
+1431 YONGE STREET
+YONGE &amp; ST CLAIR
+TORONTO, ON
+M4T 1Y7
+647 786 4344 (MAIN NUMBER)
+416 474 4786
+TIMINGS:
+MONDAY - FRIDAY: 8AM - 8PM
+WEEKENDS: 10AM - 7PM</t>
+  </si>
+  <si>
+    <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
+Best Price, Best Quality
+Buy with Confidence from our store! ✨
+---------------------------------------------
+Apple AirPods Max Hеadphones
+------------------------------------------------------------------------------------
+Apрle AirPods Max Over-Ear Noise Cancelling Bluetooth Headphones
+(Brand New in Box with 1 Year Apple Warranty)
+Price - $695 (CASH NO TAX)
+------------------------------------------------------------------------------------
+Same day delivery available in GTA arеa - delivery charges are extra dеpends on location
+------------------------------------------------------------------------------------
+BUY NOW. PAY LATER.
+Gеt easy monthly financing when you shop with Canadian Outlet
+Split your purchase into stress-freе, automatic installments with monthly Plans for:-
+3 Months
+6 Months
+12 Months
+*All financing done through Pay Bright
+------------------------------------------------------------------------------------
+Storefront is opеn to public 7 days a week from 10AM till 8PM
+------------------------------------------------------------------------------------
+We are providing FREE parking facility for our customers (Contaсt us)!!!!
+STORE LOCATION:
+СANADIAN OUTLET
+1431 YONGE STRЕET
+YONGE &amp; ST CLAIR
+TORONTО, ON
+M4T 1Y7
+647 786 4344 (MAIN NUMBER)
+416 474 4786
+TIMINGS:
+MONDAY - FRIDAY: 8AM - 8PM
+WEEKENDS: 10AM - 7PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
+Best Price, Best Quality 
+Buy with Confidence from our store!
+------------------------------------------------------
+Apple AirPods - AirPods Pro 2nd Gen, AirPods Pro, AirPods 2nd Gen Wired charging case, Apple Airpods 3rd Generation
+----------------------------------------------------
+Apple AirPods Pro (USB TO C 2nd generation)
+In-Ear Noise Cancelling True Wireless Earbuds with USB-C MagSafe Charging Case
+(Brand New in Box with 1 Year Apple Warranty)
+Price - $275(CASH NO TAX)
+Apple AirPods Pro (USB TO C 2nd generation)
+In-Ear Noise Cancelling True Wireless Earbuds with USB-C MagSafe Charging Case
+(Brand New Open Box with 9 months Apple Warranty)
+Price - $225 (CASH NO TAX)
+Apple AirPods Pro (2nd generation)
+In-Ear Noise Cancelling Truly Wireless Headphones with MagSafe Charging Case
+(Brand New in Box with 1 Year Apple Warranty)
+Price - $235(CASH NO TAX)
+Apple AirPods Pro (2nd generation)
+In-Ear Noise Cancelling Truly Wireless Headphones with MagSafe Charging Case
+(Like New in Box with Warranty)
+Price - $195 (CASH NO TAX)
+Apple AirPods Pro
+(Like New in Box with Warranty)
+Price - $175 (CASH NO TAX)
+----------------------------------------------------
+Apple Airpods 3rd Generation
+(Like New in Box with Warranty)
+Price - $160(CASH NO TAX)
+----------------------------------------------------
+Apple AirPods 2nd Generation
+In-Ear Truly Wireless Headphones with Wireless Charging Case
+(Brand New in Box with 1 Year Apple Warranty)
+Price - $175 (CASH NO TAX)
+----------------------------------------------------
+Apple AirPods Wired Earphones 2nd Generation with Charging Case
+(Brand New in Box with 1 Year Apple Warranty)
+Price - $145 (CASH NO TAX)
+Apple AirPods Wired Earphones 2nd Generation
+(Like New in Box with Warranty)
+Price - $120 (CASH NO TAX)
+----------------------------------------------------
+Same day delivery available in GTA area - delivery charges are extra depends on location
+----------------------------------------------------
+BUY NOW. PAY LATER.
+Get easy monthly financing when you shop with Canadian Outlet
+Split your purchase into stress-free, automatic installments with monthly Plans for:-
+3 Months
+6 Months
+12 Months
+*All financing done through Pay Bright*
+-------------------------------------------------------------------
+Storefront is open to public 7 days a week
+-------------------------------------------------------------------
+We are providing FREE parking facility for our customers (Contact us)!!
+-------------------------------------------------------------------
+STORE LOCATION:
+CANADIAN OUTLET
+1431 YONGE STREET
+YONGE &amp; ST CLAIR
+TORONTO, ON
+M4T 1Y7
+647 786 4344 (MAIN NUMBER)
+416 474 4786
+TIMINGS:
+MONDAY - FRIDAY: 8AM - 8PM
+WEEKENDS: 10AM - 7PM
+</t>
+  </si>
+  <si>
+    <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
+Best Price, Best Quality
+Buy with Confidence from our store! ✨
+---------------------------------------------------------------------------------------------------
+Samsung Smart TV
+------------------------------------------------------
+Samsung 75" QN800A Neo QLED 8K Smart TV (QN75QN800B)
+(NEW OPEN BOX WITH WARRANTY)
+Minоr Blemish on Screen (Not Visible)
+REGULAR PRICЕ: $4499.99 + TAX
+OUR PRICE - $1095 (CASH NO TAX)
+------------------------------------------------------
+Samsung 75" 4K UHD HDR QLED Tizen Smart TV (QN75Q70A)
+(NEW OPEN BOX WITH WARRANTY)
+REGULAR PRICE: $1799.99 + TAX
+ОUR PRICE - $895 (CASH NO TAX)
+------------------------------------------------------
+BUY NOW. PАY LATER.
+Get easy monthly financing when you shop with Canadian Outlet
+Split your purchase intо stress-free, automatic installments with monthly Plans for:-
+3 Months
+6 Months
+12 Months
+*Аll financing done through Pay Bright
+---------------------------------------------
+Same day delivеry available in GTA area - delivery charges are extra depends on location
+---------------------------------------------
+Storefront is open to publiс 7 days a week from 10AM till 8PM
+---------------------------------------------
+We are providing FREE parking facility for our customers (Contact us)!!!!
+OPEN EVERYDAY FROM 8AM TILL 8PM
+CANADIAN OUTLET
+1431 YONGE STREET
+YONGE &amp; ST CLAIR
+TORОNTO, ON
+M4T 1Y7
+647 786 4344 (MAIN NUMBER)
+4164744786
+TIMINGS:
+MONDAY - FRIDAY: 8AM - 8PM
+WЕEKENDS: 10AM - 7PM</t>
+  </si>
+  <si>
+    <t>Apple AirPods - AirPods Pro 2nd Gen, AirPods 2nd Gen, 3rd Gen</t>
+  </si>
+  <si>
+    <t>Samsung Tablets - Samsung Tab S9+, S9 FE, FE+, S9 Ultra, S6 Lite</t>
+  </si>
+  <si>
+    <t>Ecohouzng Tower Air Cooler with Humidity, 41-inches</t>
+  </si>
+  <si>
+    <t>Arctic King Window Air Conditioner 10000 BTU</t>
+  </si>
+  <si>
+    <t>Dyson Vacuums - Gen5 Outsize, Gen5 Detect, V15 Detect, DC77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10000 BTU Air Conditioners - Arctic King, KoolKing </t>
+  </si>
+  <si>
+    <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
+Best Price, Best Quality
+Buy with Confidence from our store! ✨
+----------------------------------------------------
+CELLULAR + WIFI
+----------------------------------------------------
+Samsung Tab S9 FE 5G (Wi-Fi + LTE)
+(OPEN BOX WITH WARRANTY)
+- 10.9" Display
+- 128GB Storage
+Price - $495 (CASH NO TAX)
+-----------------------------------------------------
+WIFI
+-----------------------------------------------------
+Samsung Galaxy Tab S9 Ultra 14.6" 512GB Android Tablet with Snapdragon Gen 2 Processor (CANADIAN MODEL)
+(BRAND NEW IN BOX WITH 1 YEAR SAMSUNG WARRANTY)
+- 14.6" Display
+- 512GB Stоrage
+- 12GB RAM
+Price - $1195 (CASH NО TAX)
+Samsung Galaxy Tab S9 ULTRA (Wi-Fi) With Keyboard Case (which is worth $150 for Free)(International Model)
+(BRAND NEW IN BOX WITH 1-Year WARRANTY)
+- 14.6" Display
+- 512GB Storage
+- 12GB RAM
+Price - $1195 (CASH NO TAX)
+Samsung Galaxy Tab S9 ULTRA (Wi-Fi) With Keyboard Case (which is worth $150 for Free)(International Model)
+(BRAND NEW IN BOX WITH 1-Year WARRANTY)
+- 14.6" Display
+- 256GB Storage
+- 12GB RAM
+Price - $1095 (CASH NO TAX)
+----------------------------------------------------
+Samsung Galaxy Tab S9+ (Wi-Fi) X810 (Canadian Model)
+(NEW IN BOX WITH SAMSUNG WARRANTY )
+-12.4'  Display
+- 512GB Storage
+- 12GB RAM
+Price - $1095 (CASH NO TAX)
+Samsung Galaxy Tab S9+ (Wi-Fi) X810 With Keyboard Case (which is worth $150 for Free)(International Model)
+(BRAND NEW IN BOX WITH 1 YEAR WARRANTY )
+-12.4'  Display
+- 512GB Storage
+- 12GB RAM
+Price - $1045 (CASH NO TAX)
+----------------------------------------------------
+Samsung Galaxy Tab S9 X710 (Wi-Fi) (Canadian Model)
+(NEW IN BOX WITH SAMSUNG WARRANTY)
+- 11" Display
+- 256GB Storage
+- 12GB RAM
+Price - $895 (CASH NO TAX)
+Samsung Galaxy Tab S9 X710 (Wi-Fi) With Keyboard Case (which is worth $150 for Free)(International Model)
+(BRAND NEW IN BOX WITH 1 YEAR WARRANTY)
+- 11" Display
+- 256GB Storage
+- 12GB RAM
+Price - $795(CASH NO TAX)
+----------------------------------------------------
+Samsung Tab S9 FE+ (WiFi)
+(BRAND NEW IN BOX WITH WARRANTY)
+- 12.4" Display
+- 256GB Storage
+- 12GB RAM
+Price - $695 (CASH NO TAX)
+----------------------------------------------------
+Samsung Tab S9 FE (WiFi)
+(BRAND NEW IN BOX WITH WARRANTY)
+- 10.9" Display
+- 128GB Storage
+- 6GB RAM
+Price - $395 (CASH NO TAX)
+----------------------------------------------------
+Samsung Galaxy Tab S6 Lite P613 (Wi-Fi)
+(BRAND NEW IN BOX WITH 1 YEAR WARRANTY)
+- 10.4" Display
+- 128GB Storage
+- 4GB RAM
+Price - $345(CASH NO TAX)
+Samsung Galaxy Tab S6 Lite P613 (Wi-Fi)
+(BRAND NEW IN BOX WITH 1 YEAR SAMSUNG WARRANTY)
+- 10.4" Display
+- 64GB Stоrage
+- 4GB RAM
+Price - $325(CASH NO TAX)
+----------------------------------------------------
+Same day delivery available in GTA area -delivery charges are extra depends on location
+----------------------------------------------------
+BUY NOW. PAY LATER.
+Get easy monthly financing when you shop with Canadian Outlet
+Split your purchase into stress-free, automatic installments with monthly Plans for :-
+3 Months
+6 Months
+12 Months
+*All financing done through Pay Bright
+----------------------------------------------------
+Storefront is open to public 7 days a week
+----------------------------------------------------
+We are providing a FREE parking facility for our customers (Contact us)!!
+----------------------------------------------------
+STORE LOCATION:
+CANADIAN OUTLET
+1431 YONGE STREET
+YONGE &amp; ST СLAIR
+TORONTO, ON
+M4T 1Y7
+647 786 4344 (MAIN NUMBER)
+4164744786
+TIMINGS:
+MONDAY - FRIDAY: 8AM - 8PM
+WEEKENDS: 10AM - 7PM</t>
+  </si>
+  <si>
     <t>Shop Smart, Shop Secure: Canadian Outlеt, Your Trusted Choice!
 Best Price, Best Quality
 Buy with Confidence from our store!
@@ -11732,6 +13440,10 @@
 (LIKE NEW IN BOX WITH WARRANTY)
 PRICE - $150 (CASH NO TAX)
 -------------------------------------------
+Motorola E32 64GB 2022 (DUAL SIM)
+(OPEN BOX WITH WARRANTY)
+PRICE - $225 (CASH NO TAX)
+-------------------------------------------
 MOTOROLA MOTO ONE AСE 5G 128GB
 (OPEN BOX WITH WARRANTY)
 PRICE - $175 (CASH NO TAX)
@@ -11797,1695 +13509,6 @@
 TIMINGS:
 MONDAY - FRIDAY: 8AM - 8PM
 WEEKENDS: 10AM - 7PM</t>
-  </si>
-  <si>
-    <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
-Best Price, Best Quality
-Buy with Confidence from our store! ✨
----------------------------------------------
-Samsung Phones - Samsung Galaxy A73, Samsung Galaxy A72, Samsung Galaxy A71, Samsung Galaxy A55, Samsung Galaxy A54, Samsung Galaxy A53, Samsung Galaxy A52s, Samsung Galaxy A52, Samsung Galaxy A51 Phone, Samsung A50
-BLOWOUT SALE!!!
----------------------------------------------
-Samsung Galaxy A73 128GB/6GB RAM (Dual Sim)
-(Brand New In Box With Warranty)
-Pricе: $545 (Cash No Tax)
-Samsung Galaxy A72 256GB/8GB RAM (Dual Sim)
-(Brand New In Box With Wаrranty)
-Price: $540 (Cash No Tax)
----------------------------------------------
-Samsung Galaxy A71 5G 128GB/ 6GB RAM
-(Fully Functional With store Warranty)
-Price: $195 (Cash Nо Tax)
-------------------------------------------------------------------
-Samsung Galaxy A55 5G 128GB (DUAL SIM)
-(Brand New In Box With Warranty)
-Price: $470 (Cash No Tax)
-------------------------------------------------------------------
-Samsung Galaxy A54 5G 128GB (Canadiаn / US Model)
-(Brand New In Box With Warranty)
-Price: $395 (Cash No Tax)
-Samsung Galaxy A54 5G 128GB
-(New In Box With Warranty)
-Price: $370 (Cash No Tax)
-------------------------------------------------------------------
-Samsung Galaxy A53 5G 128GB
-(New In Box With Warranty)
-Price: $360 (Cash No Tax)
-------------------------------------------------------
-Samsung Galaxy A52s 5G 128GB
-(Like New in Box With Warranty)
-Price: $275 (Cash No Tax)
-------------------------------------------------------
-Samsung Galaxy A52 5G 128GB
-(New in Box With Warranty)
-Price: $250 (Cash No Tax)
-------------------------------------------------------------------
-Samsung Galaxy A51 5G 128GB
-(Like New in Box With Warranty)
-Price: $195 (Cash No Tax)
-Samsung Galаxy A51 128GB
-(Like New in Box With Warranty)
-Price: $175 (Cash No Tax)
-Samsung Galaxy A51 64GB
-(Like New in Box With Warranty)
-Price: $150 (Cash No Tax)
-------------------------------------------------------------------
-Samsung Galaxy A50 64GB
-(Like New In Box With Warranty)
-Price: $175 (Cash No Tax)
-------------------------------------------------------------------
-Same day delivery available in GTA area -delivery charges are extra depends on location
-------------------------------------------------------------------
-BUY NOW. PAY LАTER.
-Get easy monthly financing when you shoр with Canadian Outlet
-Split your purchase into stress-free, automatic installments with monthly Plans for:-
-3 Months
-6 Months
-12 Months
-*All financing done through Pay Bright
--------------------------------------------------------------------
-Storefront is open to public 7 days a week
--------------------------------------------------------------------
-We are providing FREE parking facility for our customers (Contаct us)!!
--------------------------------------------------------------------
-STORE LOCATION:
-CANADIAN OUTLET
-1431 YONGE STREET
-YONGE &amp; ST CLAIR
-TORONTO, ON
-M4T 1Y7
-647 786 4344 (MАIN NUMBER)
-4164744786
-TIMINGS:
-MONDAY - FRIDAY: 8AM - 8PM
-WEEKENDS: 10AM - 7PM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
-Best Price, Best Quality 
-Buy with Confidence from our store! ✨
-------------------------------------------------------
-Arctic King Window Air Conditioner - 10000 BTU - 450 sq ft (MWHUK10CRN8BCL0)
-(BRAND NEW IN BOX WITH 1 YEAR MANUFACTURER WARRANTY)
-REGULAR PRICE: $469 + TAX
-OUR PRICE: $375 (CASH NO TAX)
-------------------------------------------------------
-BUY NOW. PAY LATER.
-Get easy monthly financing when you shop with Canadian Outlet
-Split your purchase into stress-free, automatic installments with monthly Plans for:-
-3 Months
-6 Months
-12 Months
-*All financing done through Pay Bright
-------------------------------------------------------
-Same day delivery available in GTA area - delivery charges are extra depends on location
-------------------------------------------------------
-Storefront is open to public 7 days a week
-------------------------------------------------------
-We are providing FREE parking facility for our customers (Contact us)!!
-------------------------------------------------------
-STORE LOCATION:
-CANADIAN OUTLET
-1431 YONGE STREET
-YONGE &amp; ST CLAIR
-TORONTO, ON
-M4T 1Y7
-647 786 4344 (MAIN NUMBER)
-416 474 4786
-TIMINGS:
-MONDAY - FRIDAY: 8AM - 8PM
-WEEKENDS: 10AM - 7PM
-</t>
-  </si>
-  <si>
-    <t>Arctic King Window AC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8000 BTU Air Conditioners - Arctic King, OmniMax, Forest Air </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
-Best Price, Best Quality 
-Buy with Confidence from our store! ✨
-------------------------------------------------------
-Forest Air 3-in-1 Portable Air Conditioner - 8000 BTU - 200-250 sq ft (A01908KR)
-(BRAND NEW IN BOX WITH 1 YEAR MANUFACTURER WARRANTY)
-REGULAR PRICE: $445.50 + TAX
-OUR PRICE: $345 (CASH NO TAX)
-------------------------------------------------------
-OMNIMAX 3-in-1 Portable Air Conditioner - 8000 BTU - 150 sq ft (OP08N3WBA1RCM)
-(BRAND NEW IN BOX WITH 1 YEAR MANUFACTURER WARRANTY)
-REGULAR PRICE: $449.99 + TAX
-OUR PRICE: $345 (CASH NO TAX)
-------------------------------------------------------
-Arctic King Portable Air Conditioner - 8000 BTU - 150 sq ft (AP53SEWBA1RCM)
-(BRAND NEW IN BOX WITH 1 YEAR MANUFACTURER WARRANTY)
-REGULAR PRICE: $379 + TAX
-OUR PRICE: $325 (CASH NO TAX)
-------------------------------------------------------
-BUY NOW. PAY LATER.
-Get easy monthly financing when you shop with Canadian Outlet
-Split your purchase into stress-free, automatic installments with monthly Plans for:-
-3 Months
-6 Months
-12 Months
-*All financing done through Pay Bright
-------------------------------------------------------
-Same day delivery available in GTA area - delivery charges are extra depends on location
-------------------------------------------------------
-Storefront is open to public 7 days a week
-------------------------------------------------------
-We are providing FREE parking facility for our customers (Contact us)!!
-------------------------------------------------------
-STORE LOCATION:
-CANADIAN OUTLET
-1431 YONGE STREET
-YONGE &amp; ST CLAIR
-TORONTO, ON
-M4T 1Y7
-647 786 4344 (MAIN NUMBER)
-416 474 4786
-TIMINGS:
-MONDAY - FRIDAY: 8AM - 8PM
-WEEKENDS: 10AM - 7PM
-</t>
-  </si>
-  <si>
-    <t>8000 BTU AC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
-Best Price, Best Quality 
-Buy with Confidence from our store! ✨
-------------------------------------------------------
-Arctic King Portable Air Conditioner - 10000 BTU - 300 sq ft (AP07SEWBA1RCM) 
-(BRAND NEW IN BOX WITH 1 YEAR MANUFACTURER WARRANTY)
-REGULAR PRICE: $549 + TAX
-OUR PRICE: $395 (CASH NO TAX)
-------------------------------------------------------
-KOOLKING Portable Air Conditioner - 10000 BTU - 540 sq ft
-(BRAND NEW IN BOX WITH 1 YEAR MANUFACTURER WARRANTY)
-REGULAR PRICE: $499.99 + TAX
-OUR PRICE: $395 (CASH NO TAX)
-------------------------------------------------------
-BUY NOW. PAY LATER.
-Get easy monthly financing when you shop with Canadian Outlet
-Split your purchase into stress-free, automatic installments with monthly Plans for:-
-3 Months
-6 Months
-12 Months
-*All financing done through Pay Bright
-------------------------------------------------------
-Same day delivery available in GTA area - delivery charges are extra depends on location
-------------------------------------------------------
-Storefront is open to public 7 days a week
-------------------------------------------------------
-We are providing FREE parking facility for our customers (Contact us)!!
-------------------------------------------------------
-STORE LOCATION:
-CANADIAN OUTLET
-1431 YONGE STREET
-YONGE &amp; ST CLAIR
-TORONTO, ON
-M4T 1Y7
-647 786 4344 (MAIN NUMBER)
-416 474 4786
-TIMINGS:
-MONDAY - FRIDAY: 8AM - 8PM
-WEEKENDS: 10AM - 7PM
-</t>
-  </si>
-  <si>
-    <t>10000 BTU AC</t>
-  </si>
-  <si>
-    <t>Arctic King, Hisense Air Conditioner - 13500 BTU, 13000BTU, 12000BTU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
-Best Price, Best Quality 
-Buy with Confidence from our store! ✨
-------------------------------------------------------
-Arctic King 3-in-1 Portable Air Conditioner - 13500 BTU - 450 sq ft (AP10SEWBA1RCM)
-(BRAND NEW IN BOX WITH 1 YEAR MANUFACTURER WARRANTY)
-REGULAR PRICE: $689 + TAX
-OUR PRICE: $545 (CASH NO TAX)
-------------------------------------------------------
-Hisense 3-in-1 Portable Smart Air Conditioner - 13000 BTU - 450 sq ft (AP1022CW1G)
-(BRAND NEW IN BOX WITH 1 YEAR MANUFACTURER WARRANTY)
-REGULAR PRICE: $697 + TAX
-OUR PRICE: $545 (CASH NO TAX)
-------------------------------------------------------
-Arctic King 3-in-1 Portable Air Conditioner - 12000 BTU - 350 sq ft (AP08SEWBA1RCM)
-(BRAND NEW IN BOX WITH 1 YEAR MANUFACTURER WARRANTY)
-REGULAR PRICE: $649 + TAX
-OUR PRICE: $495 (CASH NO TAX)
-------------------------------------------------------
-BUY NOW. PAY LATER.
-Get easy monthly financing when you shop with Canadian Outlet
-Split your purchase into stress-free, automatic installments with monthly Plans for:-
-3 Months
-6 Months
-12 Months
-*All financing done through Pay Bright
-------------------------------------------------------
-Same day delivery available in GTA area - delivery charges are extra depends on location
-------------------------------------------------------
-Storefront is open to public 7 days a week
-------------------------------------------------------
-We are providing FREE parking facility for our customers (Contact us)!!
-------------------------------------------------------
-STORE LOCATION:
-CANADIAN OUTLET
-1431 YONGE STREET
-YONGE &amp; ST CLAIR
-TORONTO, ON
-M4T 1Y7
-647 786 4344 (MAIN NUMBER)
-416 474 4786
-TIMINGS:
-MONDAY - FRIDAY: 8AM - 8PM
-WEEKENDS: 10AM - 7PM
-</t>
-  </si>
-  <si>
-    <t>High BTU AC</t>
-  </si>
-  <si>
-    <t>Samsung Phones - Samsung Z Fold 5, Fold 4, 3, 2, Flip 5, 4, 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
-Best Price, Best Quality 
-Buy with Confidence from our store! ✨
----------------------------------------------------
-Ecohouzng Tower Air Cooler with Humidity - 3-Speed - 41-in - (#CT500032HF)
-(LIKE NEW WITH WARRANTY)
-OUR PRICE: $95 (CASH NO TAX)
----------------------------------------------------
-BUY NOW. PAY LATER.
-Get easy monthly financing when you shop with Canadian Outlet
-Split your purchase into stress-free, automatic installments with monthly Plans for:-
-3 Months
-6 Months
-12 Months
-*All financing done through Pay Bright
-------------------------------------------------------
-Same day delivery available in GTA area - delivery charges are extra depends on location
-------------------------------------------------------
-Storefront is open to public 7 days a week
-------------------------------------------------------
-We are providing FREE parking facility for our customers (Contact us)!!
-------------------------------------------------------
-STORE LOCATION:
-CANADIAN OUTLET
-1431 YONGE STREET
-YONGE &amp; ST CLAIR
-TORONTO, ON
-M4T 1Y7
-647 786 4344 (MAIN NUMBER)
-416 474 4786
-TIMINGS:
-MONDAY - FRIDAY: 8AM - 8PM
-WEEKENDS: 10AM - 7PM
-</t>
-  </si>
-  <si>
-    <t>Ecohouzng Air Cooler</t>
-  </si>
-  <si>
-    <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
-Best Price, Best Quality 
-Buy with Confidence from our store!
----------------------------------------------
-Fitbit Watches - Fitbit Charge 2, Fitbit Sense 2, Fitbit Sense, Fitbit Versa, Fitbit Inspire 2, Fitbit Charge 5 Fitness Tracker, Fitbit Charge 6 Fitness Tracker, Fitbit Luxe, Fitbit Versa 2, Fitbit Versa 3 Health &amp; Fitness Smartwatch, Fitbit Versa 1
-BLOWOUT SALE!!!
--------------------------------------------------------------
-Fitbit Sense 2 Smartwatch
-(BRAND NEW WITH 1 YEAR FITBIT WARRANTY)
-PRICE - $225 (CASH NO TAX)
-Fitbit Sense Smartwatch
-(LIKE NEW WITH WARRANTY)
-PRICE - $125 (CASH NO TAX)
--------------------------------------------------------------
-Fitbit Versa 4 Smartwatch
-(BRAND NEW WITH 1 YEAR FITBIT WARRANTY)
-PRICE - $175 (CASH NO TAX)
-Fitbit Versa 4 Smartwatch
-(LIKE NEW WITH WARRANTY)
-PRICE - $125 (CASH NO TAX)
-Fitbit Versa 3 Health &amp; Fitness Smartwatch
-(LIKE NEW WITH WARRANTY)
-PRICE - $140 (CASH NO TAX)
-Fitbit Versa 2 Smartwatch
-(LIKE NEW WITH WARRANTY)
-PRICE - $115 (CASH NO TAX)
-Fitbit Versa Smartwatch
-(LIKE NEW WITH WARRANTY)
-PRICE - $70 (CASH NO TAX)
--------------------------------------------------------------
-Fitbit Charge 6 Fitness Tracker
-(LIKE NEW WITH WARRANTY)
-PRICE - $130 (CASH NO TAX)
-Fitbit Charge 5 Fitness Tracker
-(BRAND NEW IN BOX WITH WARRANTY)
-PRICE - $125(CASH NO TAX)
-Fitbit Charge 4 Fitness Tracker
-(LIKE NEW WITH WARRANTY)
-PRICE - $115 (CASH NO TAX)
-Fitbit Charge 2 Fitness Tracker
-(LIKE NEW WITH WARRANTY)
-PRICE - $55 (CASH NO TAX)
--------------------------------------------------------------
-Fitbit Luxe Fitness and Wellness Tracker
-(LIKE NEW WITH WARRANTY)
-PRICE - $75 (CASH NO TAX)
--------------------------------------------------------------
-Fitbit Inspire 2 Fitness Tracker with 24/7 Heart Rate 
-(BRAND NEW WITH 1 YEAR FITBIT WARRANTY)
-PRICE - $65 (CASH NO TAX)
--------------------------------------------------------------
-Same day delivery available in GTA area - delivery charges are extra depends on location
-----------------------------------------------------
-BUY NOW. PAY LATER.
-Get easy monthly financing when you shop with Canadian Outlet
-Split your purchase into stress-free, automatic installments with monthly Plans for:-
-3 Months
-6 Months
-12 Months
-*All financing done through Pay Bright
--------------------------------------------------------------------
-Storefront is open to public 7 days a week
--------------------------------------------------------------------
-We are providing FREE parking facility for our customers (Contact us)!!
--------------------------------------------------------------------
-STORE LOCATION:
-CANADIAN OUTLET
-1431 YONGE STREET
-YONGE &amp; ST CLAIR
-TORONTO, ON
-M4T 1Y7
-647 786 4344 (MAIN NUMBER)
-416 474 4786
-TIMINGS:
-MONDAY - FRIDAY: 8AM - 8PM
-WEEKENDS: 10AM - 7PM</t>
-  </si>
-  <si>
-    <t>JBL Speakers - JBL Clip 4, JBL Flip 6, JBL Charge 5</t>
-  </si>
-  <si>
-    <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
-Best Price, Best Quality
-Buy with Confidence from our store! ✨
----------------------------------------------
-JBL Bluetooth Speakers - JBL Charge 5, JBL Flip 6, JBL Clip 4 Bluetooth Speakers
-----------------------------------------------------
-JBL Charge 5 Waterproof Bluetooth Wireless Speaker
-(BRAND NEW IN BOX WITH WARRANTY)
-Price - $185 (CASH NO TАX)
-JBL Flip 6 Waterproof Bluetooth Wirelеss Speaker
-(BRAND NEW IN BOX WITH WARRANTY)
-Price - $135 (CASH NO TAX)
-JBL Clip 4 Waterproof Bluetooth Wireless Speaker
-(BRAND NEW IN BOX WITH WARRANTY)
-Price - $75 (CASH NO TAX)
-------------------------------------------------------
-Same day delivery available in GTA аrea - delivery charges are extra depends upоn location
-------------------------------------------------------
-BUY NOW. PAY LATER.
-Get easy monthly financing when you shop with Canadian Outlet
-Split your purchase into stress-free, automatic installments with monthly Plans for -
-3 Months
-6 Months
-12 Months
-*All financing done through PayBright
--------------------------------------------------------------------
-Storefront is open to public 7 days a week
--------------------------------------------------------------------
-We are providing FREE parking facility for our customers (Contact us)!!
--------------------------------------------------------------------
-STORE LOCATION:
-СANADIAN OUTLET
-1431 YONGE STREET
-YONGE &amp; ST CLAIR
-TORONTO, ON
-M4T 1Y7
-647 786 4344 (MAIN NUMBER)
-4164744786
-TIMINGS:
-MONDAY - FRIDAY: 8AM - 8PM
-WEEKENDS: 10AM - 7PM</t>
-  </si>
-  <si>
-    <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choiсe!
-Best Price, Best Quality
-Buy with Confidence from оur store! ✨
-------------------------------------------------------
-Samsung Phones - Samsung A35 5G, Samsung A34 5G, Samsung A33 5G, Samsung A31 phone
-BLOWOUT SALE!!!
-----------------------------------------------------------
-Samsung Galaxy A35 5G 128GB (Dual Sim)
-(Brand New In Box With Warranty)
-Price: $370 (Cash No Tax)
-----------------------------------------------------------
-Samsung Galaxy A34 5G 128GB (Dual Sim)
-(Brand New In Box With Warranty)
-Price: $335 (Cash No Tax)
-----------------------------------------------------------
-Samsung Galaxy A33 5G 128GB (Dual Sim)
-(Brand New In Box With Warranty)
-Price: $325 (Cash No Tax)
-----------------------------------------------------------
-Samsung Galaxy A31 64GB (Dual Sim)
-(Brand New In Box With Warranty)
-Price: $225 (Cash No Tax)
-----------------------------------------------------------
-Same day delivery available in GTА area-delivery charges are extra depends on location
-----------------------------------------------------------
-BUY NOW. PAY LATER.
-Get easy monthly financing when you shoр with Canadian Outlet
-Split your purchase into stress-free, automatic installments with monthly Plans for:-
-3 Mоnths
-6 Months
-12 Months
-*All financing done through Pаy Bright
--------------------------------------------------------------------
-Storefront is open to public 7 days а week
--------------------------------------------------------------------
-We are providing FREE parking facility for our customers (Contact us)!!
--------------------------------------------------------------------
-STORE LOCATION:
-CANADIAN OUTLET
-1431 YONGE STREET
-YONGE &amp; ST CLAIR
-TОRONTO, ON
-M4T 1Y7
-647 786 4344 (MAIN NUMBER)
-4164744786
-TIMINGS:
-MONDAY - FRIDAY: 8AM - 8PM
-WEEKENDS: 10AM - 7PM</t>
-  </si>
-  <si>
-    <t>50-60</t>
-  </si>
-  <si>
-    <t>50-61</t>
-  </si>
-  <si>
-    <t>50-62</t>
-  </si>
-  <si>
-    <t>50-63</t>
-  </si>
-  <si>
-    <t>50-64</t>
-  </si>
-  <si>
-    <t>50-65</t>
-  </si>
-  <si>
-    <t>50-66</t>
-  </si>
-  <si>
-    <t>50-67</t>
-  </si>
-  <si>
-    <t>50-68</t>
-  </si>
-  <si>
-    <t>50-69</t>
-  </si>
-  <si>
-    <t>50-70</t>
-  </si>
-  <si>
-    <t>50-71</t>
-  </si>
-  <si>
-    <t>50-72</t>
-  </si>
-  <si>
-    <t>70-76</t>
-  </si>
-  <si>
-    <t>70-77</t>
-  </si>
-  <si>
-    <t>70-78</t>
-  </si>
-  <si>
-    <t>samsung</t>
-  </si>
-  <si>
-    <t>Macbook Air - 13 Inch, 8GB RAM, 256GB STORAGE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
-Best Price, Best Quality 
-Buy with Confidence from our store! ✨
-------------------------------------------------------
-------------------------------------------------------
-BUY NOW. PAY LATER.
-Get easy monthly financing when you shop with Canadian Outlet
-Split your purchase into stress-free, automatic installments with monthly Plans for:-
-3 Months
-6 Months
-12 Months
-*All financing done through Pay Bright
-------------------------------------------------------
-Same day delivery available in GTA area - delivery charges are extra depends on location
-------------------------------------------------------
-Storefront is open to public 7 days a week
-------------------------------------------------------
-We are providing FREE parking facility for our customers (Contact us)!!
-------------------------------------------------------
-STORE LOCATION:
-CANADIAN OUTLET
-1431 YONGE STREET
-YONGE &amp; ST CLAIR
-TORONTO, ON
-M4T 1Y7
-647 786 4344 (MAIN NUMBER)
-416 474 4786
-TIMINGS:
-MONDAY - FRIDAY: 8AM - 8PM
-WEEKENDS: 10AM - 7PM
-</t>
-  </si>
-  <si>
-    <t>Macbook Air 8-256</t>
-  </si>
-  <si>
-    <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
-Best Price, Best Quality 
-Buy with Confidence from our store!
-------------------------------------------------------
-Dell Laptops Intel i5 - Dell inspiron 13, Dell 7480, Dell Latitude 7390, Dell Latitude 7420, Dell 5400, Dell Latitude 7400, Dell 7490, Dell 5490, Dell 3400, Dell 7480, Dell 5470 
-------------------------------------------------------
-Dell Latitude 7420 - 14" Touch
-INTEL i5 - 11th Generation
-16GB RAM
-256GB SSD
-(LIKE NEW IN BOX WITH WARRANTY)
-PRICE - $545 (CASH NO TAX)
-------------------------------------------------------
-Dell inspiron 13
-Intel i5 - 8th Generation
-16GB RAM
-512GB SSD
-(LIKE NEW IN BOX WITH WARRANTY)
-PRICE - $425 (CASH NO TAX)
-------------------------------------------------------
-Dell 7480 - 14" Touch
-Intel i5 - 7th Generation
-16GB RAM
-512GB SSD
-(LIKE NEW IN BOX WITH WARRANTY)
-PRICE - $395 (CASH NO TAX)
-------------------------------------------------------
-Dell 7410 
-INTEL i5 - 10th Generation
-16GB RAM
-512GB SSD
-(LIKE NEW IN BOX WITH WARRANTY)
-PRICE - $375 (CASH NO TAX)
-------------------------------------------------------
-Dell Latitude 7390 (Touchscreen) - 13.3"
-INTEL i5 - 8th Generation
-16GB RAM
-512GB SSD
-(LIKE NEW IN BOX WITH WARRANTY)
-PRICE - $325 (CASH NO TAX) 
-------------------------------------------------------
-Dell 5400 - 14"
-Intel i5 - 8th Generation
-16GB RAM
-256GB SSD
-(LIKE NEW IN BOX WITH WARRANTY)
-PRICE - $295 (CASH NO TAX) 
-------------------------------------------------------
-Dell Latitude 7400 - 14" Webcam
-INTEL i5 - 8th Generation
-16GB RAM
-256GB SSD
-(LIKE NEW IN BOX WITH WARRANTY)
-PRICE - $275 (CASH NO TAX)
-------------------------------------------------------
-Dell 5490 (Touchscreen)- 14"
-Intel i5 - 8th Generation
-8GB RAM
-256GB SSD
-(LIKE NEW IN BOX WITH WARRANTY)
-PRICE - $275 (CASH NO TAX)
------------------------------------------
-Dell 3400 - 14" Webcam
-Intel i5 - 8th Generation
-8GB RAM
-256GB SSD
-(LIKE NEW IN BOX WITH WARRANTY)
-PRICE - $250(CASH NO TAX)
------------------------------------------
-Dell 7490 - 14"
-Intel i5 - 8th Generation
-8GB RAM
-256GB SSD
-(LIKE NEW IN BOX WITH WARRANTY)
-PRICE - $245 (CASH NO TAX)
-Dell 7490 - 14"
-Intel i5 - 7th Generation
-16GB RAM
-256GB SSD
-(LIKE NEW IN BOX WITH WARRANTY)
-PRICE - $225 (CASH NO TAX) 
------------------------------------------
-Dell 7480 - 14"
-Intel i5 - 7th Generation
-16GB RAM
-256GB SSD
-(LIKE NEW IN BOX WITH WARRANTY)
-PRICE - $225 (CASH NO TAX)
------------------------------------------
-Dell 7480 - 14"
-Intel i5 - 6th Generation
-8GB RAM
-256GB SSD
-(LIKE NEW IN BOX WITH WARRANTY)
-PRICE - $195 (CASH NO TAX) (SOLD OUT)
------------------------------------------
-Dell 5470 14"
-Intel i5 - 6th Generation
-8GB RAM
-256GB SSD
-(LIKE NEW IN BOX WITH WARRANTY)
-PRICE - $195(CASH NO TAX) (SOLD OUT)
------------------------------------------
-Same day delivery available in GTA area -delivery charges are extra depends on location
------------------------------------------
-BUY NOW. PAY LATER.
-Get easy monthly financing when you shop with Canadian Outlet
-Split your purchase into stress-free, automatic installments with monthly Plans for:-
-3 Months
-6 Months
-12 Months
-*All financing done through Pay Bright
--------------------------------------------------------------------
-Storefront is open to public 7 days a week
--------------------------------------------------------------------
-We are providing FREE parking facility for our customers (Contact us)!!
--------------------------------------------------------------------
-STORE LOCATION:
-CANADIAN OUTLET
-1431 YONGE STREET
-YONGE &amp; ST CLAIR
-TORONTO, ON
-M4T 1Y7
-647 786 4344 (MAIN NUMBER)
-416 474 4786
-TIMINGS:
-MONDAY - FRIDAY: 8AM - 8PM
-WEEKENDS: 10AM - 7PM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Apple iPhone 15 128GB BRAND NEW </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
-Best Price, Best Quality 
-Buy with Confidence from our store! ✨
-------------------------------------------------------
-Apple iPhone 15 128GB
-(BRAND NEW WITH APPLE WARRANTY)
-PRICE - $975 (CASH NO TAX)
-------------------------------------------------------
-BUY NOW. PAY LATER.
-Get easy monthly financing when you shop with Canadian Outlet
-Split your purchase into stress-free, automatic installments with monthly Plans for:-
-3 Months
-6 Months
-12 Months
-*All financing done through Pay Bright
-------------------------------------------------------
-Same day delivery available in GTA area - delivery charges are extra depends on location
-------------------------------------------------------
-Storefront is open to public 7 days a week
-------------------------------------------------------
-We are providing FREE parking facility for our customers (Contact us)!!
-------------------------------------------------------
-STORE LOCATION:
-CANADIAN OUTLET
-1431 YONGE STREET
-YONGE &amp; ST CLAIR
-TORONTO, ON
-M4T 1Y7
-647 786 4344 (MAIN NUMBER)
-416 474 4786
-TIMINGS:
-MONDAY - FRIDAY: 8AM - 8PM
-WEEKENDS: 10AM - 7PM
-</t>
-  </si>
-  <si>
-    <t>iPhone 15</t>
-  </si>
-  <si>
-    <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
-Best Price, Best Quality
-Buy with Confidence from our store!
-------------------------------------------------------
-Samsung Phones - A15, A14, A13, A12, A11, A10S, A10E
-------------------------------------------------------
-Samsung Galaxy A15 5G 128GB/ 6GB (Dual SIM)
-(Brand New In Box With Warranty)
-Price - $210 (Cash No Tax)
-Samsung Galaxy A15 5G 128GB (Dual SIM)
-(Like New In Box With Warranty)
-Price - $180 (Cash No Tax)
-------------------------------------------------------
-Samsung Galaxy A15 128GB (Dual SIM)
-(Brand New In Box With Warranty)
-Price - $165 (Cash No Tax)
-------------------------------------------------------
-Samsung Galaxy A14 128GB (Dual SIM)
-(New In Box With Warranty)
-Price - $165 (Cash No Tax)
-Samsung Galaxy A14 64GB (Dual SIM)
-(New In Box With Warranty)
-Price - $155 (Cash No Tax)
-Samsung Galaxy A14 5G 64GB
-(New Open Box With 6 Months Store Warranty)
-Price - $165 (Cash No Tax)
----------------------------------------------------
-Samsung Galaxy A13 4GB/128GB (Dual Sim)
-(New in Box with Warranty)
-Price: $175 (Cash No Tax)
-Samsung Galaxy A13 4GB/64GB (Dual Sim)
-(New in Box with Warranty)
-Рrice: $160 (Cash No Tax)
-Samsung Galaxy A13 5G 4GB/64GB
-(Like New in Box with Warranty)
-Price: $135 (Cash No Tax)
-------------------------------------------------------
-Samsung Galaxy A12 128GB (Dual Sim)
-(New Open Box With Warranty)
-Price: $165 (Cash No Tax)
-Samsung Galaxy A12 64GB/ 4GB RAM (Dual Sim)
-(New In Box With Warranty)
-Price: $145 (Cash No Tax)
-Samsung Galaxy A12 32GB
-(Like New In Box With Warranty)
-Price: $135 (Cash No Tax)
-------------------------------------------------------
-Samsung Galaxy A11 32GB
-(New In Box With Warranty)
-Price: $125 (Cash No Tax)
-Samsung Galaxy A11 32GB
-(Fully Functional with Warranty)
-Price: $110 (Cash No Tax)
-------------------------------------------------------
-Samsung Galaxy A10s 32GB (Dual Sim)
-(Like Nеw In Box With Warranty)
-Price: $105 (Cash No Tax)
-------------------------------------------------------
-Samsung Galaxy A10E 32GB
-(Fully Functional with Warranty)
-Price: $95 (Cash No Tax)
-------------------------------------------------------
-Same day delivery available in GTA area - delivery charges are extra depends on location
----------------------------------------------------
-BUY NOW. PAY LATER.
-Get easy mоnthly financing when you shop with Canadian Outlеt
-Split your purchase into stress-free, automаtic installments with monthly Plans for:-
-3 Mоnths
-6 Months
-12 Months
-*All financing done through Pay Bright
----------------------------------------------------
-Storefront is open to рublic 7 days a week
-----------------------------------------------------
-We are providing a FREЕ parking facility for our customers (Contact us)!!
-----------------------------------------------------
-STORE LOCATION:
-CANADIAN OUTLET
-1431 YONGE STREET
-YONGE &amp; ST CLAIR
-TORONTO, ON
-M4T 1Y7
-647 786 4344 (MAIN NUMBER)
-416 474 4786
-TIMINGS:
-MONDAY - FRIDAY: 8AM - 8PM
-WEEKENDS: 10AM - 7PM</t>
-  </si>
-  <si>
-    <t>Shop Smart, Shop Secure: Canadian Outlеt, Your Trusted Choice!
-Best Price, Best Quality
-Buy with Confidence from our store!
-------------------------------------------------------
-LG Phones - LG G7 ThinQ, LG V60 ThinQ, LG G8 ThinQ, LG V40, LG V30, LG Velvet 5G, LG Phoenix 5, K50s, V20
-BLOWOUT SALE!!!
-------------------------------------------
-LG V60 ThinQ 128GB Unlocked
-(Like New in Box with warranty)
-Price - $275 (Cash No Tax)
-------------------------------------------
-LG Velvet 5G 128GB Unlocked
-(Open Box with warranty)
-Price - $225 (Cash No Tax)
-------------------------------------------
-LG G8 ThinQ 128GB Unlocked
-(Brand New in Box with warranty)
-Price - $245 (Cash No Tax)
-LG G8 ThinQ 128GB Unlocked
-(Like New in Box with warranty)
-Price - $195 (Cash No Tax)
-------------------------------------------
-LG Stylo 6 64GB Unlocked
-(Brand new in box with warranty)
-Price - $195 (Cash No Tax)
-LG Stylo 6 64GB Unlocked
-(Like new in box with warranty)
-Price - $145 (Cash No Tax)
--------------------------------------------
-LG V40 ThinQ 64GB Unlocked
-(Like New in Box with warranty)
-Price - $175 (Cash No Tax)
-------------------------------------------
-LG V30 64GB Unlocked
-(Brand new in box with warranty)
-Price - $175 (Cash No Tax)
-------------------------------------------
-LG G7 ThinQ 64GB Unlocked
-(Like New in Box with warranty)
-Price - $165 (Cash No Tax)
-------------------------------------------
-LG V20 64GB Unlocked Smartphone
-(Like New in Box with Warranty)
-Price - $145 (Сash No Tax)
---------------------------------------------
-LG K50s 32GB Unlocked
-(Brand new in box with warranty)
-Price - $160 (Cash No Tax)
--------------------------------------------
-LG Pheonix 5 16GB Unlocked
-(Like New in Box with warranty)
-Price - $95 (Cash No Tax)
--------------------------------------------
-Same day delivery available in GTA area - delivery charges are extra depends on location
-----------------------------------------------------
-BUY NOW. PAY LATER.
-Get easy monthly financing when you shop with Canadian Outlet
-Split yоur purchase into stress-free, automatic installments with monthly Plans for:-
-3 Months
-6 Months
-12 Months
-*All financing done through Pay Bright
--------------------------------------------------------------------
-Stоrefront is open to public 7 days a week
--------------------------------------------------------------------
-We are providing FREE parking facility for our customers (Contact us)!!
--------------------------------------------------------------------
-STORE LOCATION:
-CANADIAN OUTLET
-1431 YONGE STREET
-YONGE &amp; ST CLAIR
-TORONTO, ON
-M4T 1Y7
-647 786 4344 (MAIN NUMBER)
-416 474 4786
-TIMINGS:
-MONDAY - FRIDAY: 8AM - 8PM
-WEEKENDS: 10AM - 7PM</t>
-  </si>
-  <si>
-    <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
-Best Price, Best Quality
-Buy with Confidеnce from our store!
-------------------------------------------------------
-HP Laptops Intel i5 - HP EliteBook 840 G9, HP PrоBook 440 G3, HP ELITEBOOK 840 G7, HР ELITEBOOK 840 G6, HP Probook 430 G5, HP 15 DY2795WM, HP ProBook 430 G3, HP ELITEBOOK 840 G4, HP ELITEBOOK 840 G6, HP EliteBook Folio 9470M
-------------------------------------------------------
-HP EliteBook 840 G9 - 14"
-Intel Core i5 - 12th Gen
-16GB RAM
-512GB SSD
-Intel Iris XЕ Graphics
-Windows 11 Pro
-(BRAND NЕW IN BOX WITH WARRANTY)
-PRICE - $1295 (CASH NO TAX)
-------------------------------------------------------
-HP 15 DY2795WM 15.6
-INTEL i5 - 11TH GEN
-8GB RAM
-256GB SSD
-(Brand New In Box With Warranty)
-PRICE - $595 (CASH NO TAX)
-------------------------------------------------------
-HP ELITEBOOK 840 G7 - 14"
-INTEL i5 - 10TH GEN
-16GB RAM
-256GB SSD
-(LIKE NEW IN BOX WITH WARRANTY)
-PRICE - $475 (CASH NO TAX)
-------------------------------------------------------
-HP ELITEBOOK 840 G6 - 14"
-INTEL i5 - 8TH GEN
-16GB RAM
-256GB SSD
-(LIKE NEW IN BOX WITH WARRANTY)
-PRICE - $325(CASH NO TAX)
------------------------------------------------------
-HP ProBook 430 G3 13.3" (Touchscrеen)
-INTEL i5 - 6TH GEN
-8GB RAM
-256GB SSD
-(LIKE NEW IN BOX WITH WARRАNTY)
-PRICE - $325 (CASH NO TAX)
-------------------------------------------------------
-HP ELITEBOOK 840 G6 - 14"
-INTEL i5 - 8TH GEN
-8GB RAM
-256GB SSD
-(LIKE NEW IN BОX WITH WARRANTY)
-PRICE - $295(CASH NO TAX)
-------------------------------------------------------
-HP Probook 430 G5 - 13.3"
-INTEL i5 - 8TH GEN
-16GB RAM
-256GB SSD
-(LIKE NEW IN BOX WITH WARRANTY)
-PRIСE - $275(CASH NO TAX)
-------------------------------------------------------
-Same day delivery availablе in GTA area -delivery charges are еxtra depends on location
-------------------------------------------------------
-BUY NOW. PAY LATER.
-Get easy monthly financing when you shоp with Canadian Outlet
-Split your purchase into stress-free, automatic installments with monthly Plans fоr:-
-3 Months
-6 Months
-12 Months
-*All financing done through Pay Bright
-------------------------------------------------------
-Storefront is open to public 7 days a week
-------------------------------------------------------
-We are providing FREE parking facility for our customers (Contact us)!!
-------------------------------------------------------
-STORE LOCATION:
-CANADIAN OUTLET
-1431 YONGE STREET
-YONGE &amp; ST CLAIR
-TORONTO, ON
-M4T 1Y7
-647 786 4344 (MAIN NUMBER)
-4164744786
-TIMINGS:
-MONDAY - FRIDAY: 8AM - 8PM
-WEEKENDS: 10AM - 7PM</t>
-  </si>
-  <si>
-    <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
-Best Price, Best Quality
-Buy with Confidence from our store! ✨
----------------------------------------------
-Samsung Phones - Samsung Galaxy A05s, Samsung Galaxy A05, Samsung Galaxy A04, Samsung Galaxy A04e, Samsung Galaxy A03s, Samsung Galaxy A02s, Samsung Galaxy A02, Samsung Galaxy A03 Core phone
-Samsung Galaxy A05s 128GB (Dual Sim)
-(New In Box With Warranty)
-Price: $175 (Cash No Tax)
-Samsung Galaxy A05s 64GB (Dual Sim)
-(New In Box With Warranty)
-Price: $150 (Cash Nо Tax)
-Samsung Galaxy A05 128GB (Dual Sim)
-(New In Box With Warranty)
-Price: $140 (Cash No Tax)
-Samsung Galaxy A05 64GB (Dual Sim)
-(New In Box With Warranty)
-Priсe: $135 (Cash No Tax)
----------------------------------------------
-Samsung Galaxy A04 64GB (Dual Sim)
-(New In Box With Warranty)
-Price: $135 (Cash No Tax)
-Samsung Galaxy A04 32GB (Dual Sim)
-(Nеw In Box With Warranty)
-Price: $115 (Cash No Tax)
----------------------------------------------
-Sаmsung Galaxy A04e 64GB (Dual Sim)
-(New In Box With Warranty)
-Pricе: $125 (Cash No Tax)
-Samsung Galaxy A04e 32GB (Dual Sim)
-(New In Box With Warranty)
-Price: $105 (Cash No Tax)
----------------------------------------------
-Sаmsung Galaxy A03s 32GB
-(New In Bоx With Warranty)
-Price: $125 (Cаsh No Tax)
----------------------------------------------
-Samsung Galaxy A02s 32GB (Dual Sim)
-(New In Box With Warranty)
-Price: $125 (Cash No Tax)
----------------------------------------------
-Sаmsung Galaxy A02 32GB (Dual Sim)
-(New In Box With Warranty)
-Price: $115 (Cash No Tax)
----------------------------------------------
-Samsung Galaxy A03 Core 32GB
-(New In Box With Warranty)
-Priсe: $100 (Cash No Tax)
----------------------------------------------
-Same day delivery available in GTA area -delivery charges are extra depends on location
----------------------------------------------
-BUY NOW. PAY LATER.
-Get easy monthly financing when you shop with Сanadian Outlet
-Split your purchasе into stress-free, automatic installments with monthly Plans for:-
-3 Months
-6 Months
-12 Months
-*Аll financing done through Pay Bright
--------------------------------------------------------------------
-Storefront is open to public 7 days a week
--------------------------------------------------------------------
-We are providing FREE рarking facility for our customers (Contact us)!!
--------------------------------------------------------------------
-STORE LOCATION:
-CANADIAN OUTLET
-1431 YONGE STREET
-YONGE &amp; ST CLAIR
-TORONTO, ON
-M4T 1Y7
-647 786 4344 (MAIN NUMBER)
-4164744786
-TIMINGS:
-MONDAY - FRIDAY: 8AM - 8PM
-WEEKENDS: 10AM - 7PM</t>
-  </si>
-  <si>
-    <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
-Best Price, Best Quality
-Buy with Confidence from our storе!
----------------------------------------------
-Samsung Phones - Samsung A25, Samsung A24, Samsung A23, Samsung A22, Samsung A21S
-BLOWOUT SALE!!!
----------------------------------------------
-Samsung Galaxy A25 5G 128GB (Dual Sim)
-(Brand New In Box With Warranty)
-Priсe: $250 (Cash No Tax)
----------------------------------------------------
-Samsung Galaxy А24 128GB (Dual Sim)
-(Brand Nеw In Box With Warranty)
-Pricе: $235 (Cash No Tax)
----------------------------------------------------
-Samsung Galaxy A23 128GB (Dual Sim)
-(Brand New In Box With Warranty)
-Price: $215 (Cash No Tax)
-Samsung Galaxy A23 64GB (Dual Sim)
-(Brand New In Box With Warranty)
-Price: $200 (Cash No Tax)
----------------------------------------------
-Samsung Galaxy A22 128GB (Dual Sim)
-(Brand New In Box With Warranty)
-Price: $210 (Cash No Tax)
-Samsung Galaxy A22 64GB (Dual Sim)
-(Brand New In Box With Warranty)
-Price: $200 (Cash No Tax)
-Samsung Galaxy A22 5G 64GB (Dual Sim)
-(Brand New In Box With Warranty)
-Price: $210 (Cаsh No Tax)
----------------------------------------------
-Samsung Galaxy A21S 128GB (Dual Sim)
-(Brand New In Box With Wаrranty)
-Price: $200 (Cash No Tax)
-Samsung Galaxy A21S 64GB (Dual Sim)
-(Brand New In Box With Warranty)
-Price: $190 (Cash No Tax)
----------------------------------------------
-Same day delivery availablе in GTA area - delivery charges are extra depends on location
----------------------------------------------------
-BUY NOW. PAY LATER.
-Get easy monthly finаncing when you shop with Canadiаn Outlet
-Split your purchase into stress-free, automatic installments with monthly Plans for:-
-3 Months
-6 Months
-12 Months
-*All financing done through Pay Bright
--------------------------------------------------------------------
-Storefront is open to public 7 days a week
--------------------------------------------------------------------
-We are providing FREE parking facility for our customers (Contact us)!!
--------------------------------------------------------------------
-STORE LOCАTION:
-CANADIAN OUTLET
-1431 YONGE STREET
-YONGE &amp; ST CLAIR
-TORONTO, ON
-M4T 1Y7
-647 786 4344 (MAIN NUMBER)
-4164744786
-TIMINGS:
-MONDAY - FRIDAY: 8AM - 8PM
-WEEKENDS: 10AM - 7PM</t>
-  </si>
-  <si>
-    <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
-Best Price, Best Quality
-Buy with Cоnfidence from our store!
----------------------------------------------
-BLOWOUT SALE!!!
-Samsung Gаlaxy S24 Ultra, Samsung Galaxy S24, Samsung Galaxy S23 Ultra, Samsung Galaxy S23, Samsung Galaxy S23+, Sаmsung Galaxy S23 FE, Samsung Galaxy S22 Ultra, Samsung Galaxy S22+, Sаmsung Galaxy S22
------------------------------------------------------------------------
-Samsung Galаxy S24 Ultra 12GB / 512GB (DUAL SIM)
-(Brand New in Box with 1 Year Warranty)
-Price - $1545 (CASH NО TAX)
-Samsung Galaxy S24 Ultrа 12GB / 256GB (CANADIAN MODEL)
-(Brand New Open Box with Warranty)
-Price - $1095 (CASH NO TAX)
------------------------------------------------------------------------
-Samsung Galaxy S24 256GB (CANADIAN MODEL)
-(Brand New in Box with 1 Year Samsung Warranty)
-PRICE - $825 (CASH NO TAX)
-Samsung Galaxy S24 256GB (CANADIAN MODEL)
-(Like New in Box with Warranty)
-PRICE - $750 (CASH NO TAX)
-Samsung Galaxy S24 128GB (CANADIAN MODEL)
-(Brand New in Box with 1 Year Samsung Warranty)
-PRICE - $740 (CASH NO TAX)
-Samsung Galaxy S24 128GB (CANADIAN MODEL)
-(Like New in Box with Warranty)
-PRICE - $695 (CASH NO TAX)
------------------------------------------------------------------------
-Samsung Galaxy S23 Ultra 512GB (DUAL SIM)
-(Brand New in Box with 1 Year Warranty)
-Price - $1250 (CASH NO TAX)
-Samsung Galaxy S23 Ultra 512GB
-(Like New in Box with Warranty)
-Price - $995 (CASH NO TAX)
-Samsung Galaxy S23 Ultra 256GB (DUAL SIM)
-(Brаnd New in Box with 1 Year Warranty)
-Price - $1095 (CASH NO TAX)
-Samsung Galaxy S23 Ultra 256GB
-(Like New in Box with Warranty)
-Price - $950 (CASH NO TAX)
----------------------------------------------
-Samsung Galaxy S23+ 256GB (DUAL SIM)
-(Brand New in Box with 1 Year Warranty)
-Price - $945 (CASH NO TAX)
----------------------------------------------
-Samsung Galaxy S23 256GB (CANADIAN MODEL)
-(Brand New Open Box with Samsung Warranty)
-Price - $795 (CASH NO TAX)
-Samsung Galaxy S23 128GB (CANADIAN MODEL)
-(Brand New in Box with 1 Year Samsung Warranty)
-Price - $735 (CASH NO TAX)
-Samsung Galaxy S23 5G 128GB
-(New Open Box with 6 Months Warranty)
-Price - $625 (CASH NO TAX)
----------------------------------------------
-Samsung Galaxy S23 FE 5G 256GB (DUAL SIM)
-(Brand New in Box with 1 Year Warranty)
-Price - $645 (CASH NO TAX)
-Samsung Galaxy S23 FE 5G 256GB
-(Like New in Box with Warranty)
-Price - $575 (CАSH NO TAX)
-Samsung Galaxy S23 FЕ 5G 128GB (CANADIAN MODEL)
-(Brand New in Box with 1 Year Samsung Warranty)
-Price - $595 (CASH NO TAX)
-Samsung Galaxy S23 FE 5G 128GB
-(Like New in Box with Warranty)
-Рrice - $500 (CASH NO TAX)
----------------------------------------------
-Samsung Galaxy S22 Ultra 5G 512GB
-(LIKE NEW IN BOX WITH WARRANTY)
-PRICE: $695 (CASH NO TAX)
-Samsung Galaxy S22 Ultra 5G 256GB
-(LIKE NEW IN BOX WITH WARRANTY)
-PRICE: $645 (CASH NO TAX)
-Samsung Galaxy S22 Ultra 5G 128GB
-(LIKE NEW IN BOX WITH WARRANTY)
-PRICE: $595 (CASH NO TAX)
----------------------------------------------
-Sаmsung Galaxy S22+ (Plus) 5G 256GB
-(LIKE NEW IN BOX WITH WARRANTY)
-PRICE: $495 (CASH NO TAX)
-Samsung Galaxy S22+ (Plus) 5G 128GB
-(LIKE NEW IN BOX WITH WARRANTY)
-PRICE: $445 (CASH NO TAX)
----------------------------------------------
-Samsung Galaxy S22 5G 256GB
-(LIKE NEW IN BOX WITH WARRANTY)
-PRICЕ: $395 (CASH NO TAX)
-Samsung Galaxy S22 5G 128GB
-(LIKE NEW IN BOX WITH WARRANTY)
-PRICE: $375 (CASH NO TAX)
----------------------------------------------
-Same day dеlivery available in GTA area - delivery charges are extra depends on location
-------------------------------------------------------------------------
-BUY NOW. PAY LATER.
-Get easy monthly financing when you shop with Canadian Outlet
-Sрlit your purchase into stress-free, automatic installments with monthly Plans for:-
-3 Months
-6 Months
-12 Months
-*All financing done through Pay Bright
----------------------------------------------
-Storefront is open to public 7 days a week
----------------------------------------------
-We are providing FREE parking facility for our customers (Contact us)!!
----------------------------------------------
-STORE LOCATION:
-CANADIAN OUTLЕT
-1431 YONGE STREET
-YONGE &amp; ST CLAIR
-TORONTO, ON
-M4T 1Y7
-647 786 4344 (MAIN NUMBER)
-416 474 4786
-TIMINGS:
-MONDAY - FRIDAY: 8AM - 8PM
-WEEKENDS: 10AM - 7PM</t>
-  </si>
-  <si>
-    <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
-Best Price, Best Quality
-Buy with Confidence from our store! ✨
----------------------------------------------
-JBL Harman Endurance Race, JBL Vibe Beam In-Ear Sound Isolating Truly Wireless Headphones, JBL Run 2, JBL 215 BT, JBL 125BT
----------------------------------------------------
-JBL Vibe Beam In-Ear Sound Isolating Truly Wireless Headphones
-(BRAND NEW IN BOX)
-PRICE - $70 (CASH NO TAX)                                                                                                                                                                                                                                                                                                                   
-                                                                                                                                                                                                                                                                                                                                                                                                                                            JBL Harman Endurance Race Waterproof True Wireless Active Sport Earbuds
-(BRAND NEW IN BOX)
-Price - $60 (CASH NO TAX)
-JBL Еndurance RUN 2 In-Ear Wireless Sport Headphones
-(BRAND NEW IN BOX)
-Price - $35 (CASH NO TAX)
-JBL Tune 215BT Wireless Earbud headphones
-(BRAND NEW IN BOX)
-Price - $35 (CASH NO TAX)
-JBL Tune 125BT Wireless Earbud headphones
-(BRAND NEW IN BOX)
-Price - $35 (CASH NO TAX)
----------------------------------------------------
-Same day dеlivery available in GTA area - delivery charges are extra depends on location
----------------------------------------------------
-BUY NOW. PAY LATER.
-Get easy monthly financing when you shop with Canadian Outlet
-Split your purchase into stress-free, automatic installments with monthly Plans for:-
-3 Months
-6 Months
-12 Months
-*All financing done through Pay Bright
--------------------------------------------------------------------
-Storefront is open to public 7 days a week
--------------------------------------------------------------------
-We are providing a FREE parking facility for our customers (Contact us)!!
--------------------------------------------------------------------
-STORE LOCATION:
-CANADIAN OUTLET
-1431 YONGE STREET
-YONGE &amp; ST CLAIR
-TORONTO, ON
-M4T 1Y7
-647 786 4344 (MAIN NUMBER)
-416 474 4786
-TIMINGS:
-MONDAY - FRIDAY: 8AM - 8PM
-WEEKENDS: 10АM - 7PM</t>
-  </si>
-  <si>
-    <t>ASTRO Gaming A50 Wireless Headset + Base Station</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
-Best Price, Best Quality 
-Buy with Confidence from our store! ✨
-------------------------------------------------------
-ASTRO Gaming A50 Wireless Headset + Base Station Gen 4 - Compatible With PS5, PS4, PC, Mac
-(Brand New in Box)
-Price - $260 (Cash No Tax)
-ASTRO Gaming A50 Wireless + Base Station for Xbox One and Series X &amp; PC
-(Brand New in Box)
-Price - $260 (Cash No Tax)
-------------------------------------------------------
-BUY NOW. PAY LATER.
-Get easy monthly financing when you shop with Canadian Outlet
-Split your purchase into stress-free, automatic installments with monthly Plans for:-
-3 Months
-6 Months
-12 Months
-*All financing done through Pay Bright
-------------------------------------------------------
-Same day delivery available in GTA area - delivery charges are extra depends on location
-------------------------------------------------------
-Storefront is open to public 7 days a week
-------------------------------------------------------
-We are providing FREE parking facility for our customers (Contact us)!!
-------------------------------------------------------
-STORE LOCATION:
-CANADIAN OUTLET
-1431 YONGE STREET
-YONGE &amp; ST CLAIR
-TORONTO, ON
-M4T 1Y7
-647 786 4344 (MAIN NUMBER)
-416 474 4786
-TIMINGS:
-MONDAY - FRIDAY: 8AM - 8PM
-WEEKENDS: 10AM - 7PM
-</t>
-  </si>
-  <si>
-    <t>Astro Gaming</t>
-  </si>
-  <si>
-    <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
-Best Price, Best Quality
-Buy with Confidence from our store! ✨
----------------------------------------------
-Samsung Galaxy Buds2 Pro Headphones, Samsung Galaxy Buds2 Headphones, Samsung Galaxy Buds FE, Samsung Galaxy Buds Headрhones
----------------------------------------------------
-Samsung Galaxy Buds2 Pro In-Ear Noise Сancelling Truly Wireless Headphones
-(BRAND NEW IN BOX WITH WARRANTY)
-PRICE - $145 (CASH NO TAX)
-Samsung Galaxy Buds2 In-Ear Noise Cancelling Truly Wireless Headphones
-(BRAND NEW IN BOX WITH WARRANTY)
-PRICE - $75 (CASH NO TAX)
-Samsung Galaxy Buds FE Truly Wireless Bluetooth Earbuds, Active Noise Cancellation(ANC)
-(BRAND NEW IN BOX WITH WARRANTY)
-PRICE - $85 (CASH NO TAX)
----------------------------------------------------
-Same day delivery available in GTA area - delivery charges are extra depends on loсation
----------------------------------------------------
-BUY NОW. PAY LATER.
-Get easy monthly financing when you shop with Canadian Outlet
-Split your purchаse into stress-free, automatic installments with monthly Plans for:-
-3 Months
-6 Months
-12 Months
-*All financing done through Pay Bright
----------------------------------------------------
-Storefront is open to public 7 days a week
-----------------------------------------------------
-We are providing a FREE parking facility for our customers (Contаct us)!!
-----------------------------------------------------
-STORE LOCATION:
-CANADIAN OUTLЕT
-1431 YONGE STREET
-YONGE &amp; ST CLAIR
-TORONTO, ON
-M4T 1Y7
-647 786 4344 (MAIN NUMBER)
-416 474 4786
-TIMINGS:
-MONDAY - FRIDАY: 8AM - 8PM
-WEEKENDS: 10AM - 7РM</t>
-  </si>
-  <si>
-    <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
-Best Price, Best Quality
-Buy with Confidence from our store! ✨
----------------------------------------------
-Bose QuietComfort Ultra Headphones, QuietComfort and QuietComfort 45 Bluetooth Headphones, Bose Ultra Earbuds
----------------------------------------------------
-Bose QuietComfort Ultra Wireless Noise Cancelling Headрhones
-(BRAND NEW IN BOX WITH 1 YEAR MANUFACTURER WARRANTY)
-PRICE - $445 (CASH NO TAX)
----------------------------------------------------
-Bose QuietComfort Wireless Noise Cancelling Headphones
-(BRAND NEW IN BOX WITH 1 YEAR MANUFACTURER WARRANTY)
-PRICE - $375 (CASH NO TAX)
-Bose QuietComfort 45 Over-Ear Noise Cancelling Bluetooth Headphоnes
-(BRAND NEW IN BOX WITH 1 YEAR MANUFACTURER WАRRANTY)
-PRICE - $345(CASH NO TAX)
----------------------------------------------------
-Bose QuiеtComfort Ultra Wireless Noise Cancelling Earbuds, Bluetooth Noise Cancelling Earbuds with Spatial Audio and World-Class Noise Cancellation
-(BRAND NEW IN BOX WITH WARRANTY)
-PRICE - $275 (CASH NO TAX)
----------------------------------------------------
-Bose QuietComfort Ultra Wireless Noise Cancelling Earbuds, Bluetooth Noise Cancelling Earbuds with Spatial Audio and World-Class Noise Canсellation
-(NEW OPEN BOX WITH WARRANTY)
-PRICE - $225 (CASH NO TAX)
----------------------------------------------------
-Same day delivery availаble in GTA area - delivery charges are extra depends on location
----------------------------------------------------
-BUY NOW. PAY LATER.
-Get easy monthly financing when you shop with Canadian Outlet
-Split your purchase into stress-free, automatic installments with monthly Plans for:-
-3 Mоnths
-6 Months
-12 Months
-*All financing done through Pay Bright
--------------------------------------------------------------------
-Storefront is open to public 7 days a week
--------------------------------------------------------------------
-We are providing FREE parking facility for our customers (Contact us)!!
--------------------------------------------------------------------
-STORE LOCATION:
-CANADIAN OUTLET
-1431 YONGE STREET
-YОNGE &amp; ST CLAIR
-TORONTO, ON
-M4T 1Y7
-647 786 4344 (MAIN NUMBER)
-4164744786
-TIMINGS:
-MONDAY - FRIDAY: 8AM - 8PM
-WEEKENDS: 10AM - 7PM</t>
-  </si>
-  <si>
-    <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choiсe!
-Best Price, Best Quality
-Buy with Confidence from оur store! ✨
----------------------------------------------------
-Beats Studio Pro, Beats Studio3 Headphones, Powеrbeats Pro Headphones, Beats By Dr. Dre Fit Pro, Beats Studio Buds + Earbuds, Beats Studio Buds, Powerbeats 3
----------------------------------------------------
-Beats Studio Pro - Wireless Bluetooth Noise Cancelling Headphones
-(BRAND NEW IN BOX)
-Price - $295 (Cash No Tax)
-Beats Beаts Studio3 Wireless Over-Ear Headphones
-(BRAND NEW IN BOX)
-Price - $225 (Cash No Tax)
----------------------------------------------------
-Beats Powerbeats Pro In-Ear Truly Wireless Headphones
-(BRAND NEW IN BOX)
-PRICE - $195 (CASH NO TAX)
-------------------------------------------------------
-Beats Powerbeats Pro In-Ear Truly Wireless Headphones
-(LIKE NEW IN BOX)
-PRICE - $145 (CASH NO TАX)
-------------------------------------------------------
-Beats Fit Pro X Alo Special Edition In-Ear Noise Cancеlling True Wireless Earbuds (BRAND NEW IN BOX)
-PRICE - $195 (CASH NO TAX)
-Beats Fit Pro In-Ear Noise Cancelling True Wireless Earbuds
-(BRAND NEW IN BOX)
-PRICE - $175 (CASH NO TAX)
-------------------------------------------------------
-Beats Studio Budsplus [+] True Wireless Noise Cancelling Earbuds
-(BRAND NEW IN BOX)
-PRICE - $145 (СASH NO TAX)
-------------------------------------------------------
-Beats Studio Buds In-Ear Noise Cancelling True Wireless Earbuds
-(BRAND NEW IN BOX)
-PRICE - $115 (CASH NO TAX)
-------------------------------------------------------
-Beats Studio Buds In-Ear Noise Cancelling True Wireless Earbuds
-(LIKE NEW IN BOX)
-PRICE - $85 (CASH NO TAX)
-------------------------------------------------------
-Beats Powerbeats3 Wireless in-Ear Headphones - White
-(BRAND NEW IN BOX)
-PRICE - $65 (CASH NO TAX)
-------------------------------------------------------
-Samе day delivery available in GTA area - delivery charges are extra depends on location
-------------------------------------------------------
-BUY NOW. PAY LATER.
-Get easy monthly financing when you shop with Canadian Outlet
-Split your purchase into stress-free, automatic installments with monthly Plans for:-
-3 Months
-6 Months
-12 Months
-*Аll financing done through Pay Bright
----------------------------------------------------
-Storefront is open to public 7 days a week
-----------------------------------------------------
-We are providing a FREE parking facility for our customers (Contact us)!!
-----------------------------------------------------
-STORE LOCATION:
-CANADIAN OUTLET
-1431 YONGE STREET
-YONGE &amp; ST CLAIR
-TORONTO, ON
-M4T 1Y7
-647 786 4344 (MAIN NUMBER)
-416 474 4786
-TIMINGS:
-MONDAY - FRIDAY: 8AM - 8PM
-WEEKENDS: 10AM - 7PM</t>
-  </si>
-  <si>
-    <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
-Best Price, Best Quality
-Buy with Confidence from our store! ✨
----------------------------------------------
-Apple AirPods Max Hеadphones
-------------------------------------------------------------------------------------
-Apрle AirPods Max Over-Ear Noise Cancelling Bluetooth Headphones
-(Brand New in Box with 1 Year Apple Warranty)
-Price - $695 (CASH NO TAX)
-------------------------------------------------------------------------------------
-Same day delivery available in GTA arеa - delivery charges are extra dеpends on location
-------------------------------------------------------------------------------------
-BUY NOW. PAY LATER.
-Gеt easy monthly financing when you shop with Canadian Outlet
-Split your purchase into stress-freе, automatic installments with monthly Plans for:-
-3 Months
-6 Months
-12 Months
-*All financing done through Pay Bright
-------------------------------------------------------------------------------------
-Storefront is opеn to public 7 days a week from 10AM till 8PM
-------------------------------------------------------------------------------------
-We are providing FREE parking facility for our customers (Contaсt us)!!!!
-STORE LOCATION:
-СANADIAN OUTLET
-1431 YONGE STRЕET
-YONGE &amp; ST CLAIR
-TORONTО, ON
-M4T 1Y7
-647 786 4344 (MAIN NUMBER)
-416 474 4786
-TIMINGS:
-MONDAY - FRIDAY: 8AM - 8PM
-WEEKENDS: 10AM - 7PM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
-Best Price, Best Quality 
-Buy with Confidence from our store!
-------------------------------------------------------
-Apple AirPods - AirPods Pro 2nd Gen, AirPods Pro, AirPods 2nd Gen Wired charging case, Apple Airpods 3rd Generation
-----------------------------------------------------
-Apple AirPods Pro (USB TO C 2nd generation)
-In-Ear Noise Cancelling True Wireless Earbuds with USB-C MagSafe Charging Case
-(Brand New in Box with 1 Year Apple Warranty)
-Price - $275(CASH NO TAX)
-Apple AirPods Pro (USB TO C 2nd generation)
-In-Ear Noise Cancelling True Wireless Earbuds with USB-C MagSafe Charging Case
-(Brand New Open Box with 9 months Apple Warranty)
-Price - $225 (CASH NO TAX)
-Apple AirPods Pro (2nd generation)
-In-Ear Noise Cancelling Truly Wireless Headphones with MagSafe Charging Case
-(Brand New in Box with 1 Year Apple Warranty)
-Price - $235(CASH NO TAX)
-Apple AirPods Pro (2nd generation)
-In-Ear Noise Cancelling Truly Wireless Headphones with MagSafe Charging Case
-(Like New in Box with Warranty)
-Price - $195 (CASH NO TAX)
-Apple AirPods Pro
-(Like New in Box with Warranty)
-Price - $175 (CASH NO TAX)
-----------------------------------------------------
-Apple Airpods 3rd Generation
-(Like New in Box with Warranty)
-Price - $160(CASH NO TAX)
-----------------------------------------------------
-Apple AirPods 2nd Generation
-In-Ear Truly Wireless Headphones with Wireless Charging Case
-(Brand New in Box with 1 Year Apple Warranty)
-Price - $175 (CASH NO TAX)
-----------------------------------------------------
-Apple AirPods Wired Earphones 2nd Generation with Charging Case
-(Brand New in Box with 1 Year Apple Warranty)
-Price - $145 (CASH NO TAX)
-Apple AirPods Wired Earphones 2nd Generation
-(Like New in Box with Warranty)
-Price - $120 (CASH NO TAX)
-----------------------------------------------------
-Same day delivery available in GTA area - delivery charges are extra depends on location
-----------------------------------------------------
-BUY NOW. PAY LATER.
-Get easy monthly financing when you shop with Canadian Outlet
-Split your purchase into stress-free, automatic installments with monthly Plans for:-
-3 Months
-6 Months
-12 Months
-*All financing done through Pay Bright*
--------------------------------------------------------------------
-Storefront is open to public 7 days a week
--------------------------------------------------------------------
-We are providing FREE parking facility for our customers (Contact us)!!
--------------------------------------------------------------------
-STORE LOCATION:
-CANADIAN OUTLET
-1431 YONGE STREET
-YONGE &amp; ST CLAIR
-TORONTO, ON
-M4T 1Y7
-647 786 4344 (MAIN NUMBER)
-416 474 4786
-TIMINGS:
-MONDAY - FRIDAY: 8AM - 8PM
-WEEKENDS: 10AM - 7PM
-</t>
-  </si>
-  <si>
-    <t>Shop Smart, Shop Secure: Canadian Outlet, Your Trusted Choice!
-Best Price, Best Quality
-Buy with Confidence from our store! ✨
----------------------------------------------------------------------------------------------------
-Samsung Smart TV
-------------------------------------------------------
-Samsung 75" QN800A Neo QLED 8K Smart TV (QN75QN800B)
-(NEW OPEN BOX WITH WARRANTY)
-Minоr Blemish on Screen (Not Visible)
-REGULAR PRICЕ: $4499.99 + TAX
-OUR PRICE - $1095 (CASH NO TAX)
-------------------------------------------------------
-Samsung 75" 4K UHD HDR QLED Tizen Smart TV (QN75Q70A)
-(NEW OPEN BOX WITH WARRANTY)
-REGULAR PRICE: $1799.99 + TAX
-ОUR PRICE - $895 (CASH NO TAX)
-------------------------------------------------------
-BUY NOW. PАY LATER.
-Get easy monthly financing when you shop with Canadian Outlet
-Split your purchase intо stress-free, automatic installments with monthly Plans for:-
-3 Months
-6 Months
-12 Months
-*Аll financing done through Pay Bright
----------------------------------------------
-Same day delivеry available in GTA area - delivery charges are extra depends on location
----------------------------------------------
-Storefront is open to publiс 7 days a week from 10AM till 8PM
----------------------------------------------
-We are providing FREE parking facility for our customers (Contact us)!!!!
-OPEN EVERYDAY FROM 8AM TILL 8PM
-CANADIAN OUTLET
-1431 YONGE STREET
-YONGE &amp; ST CLAIR
-TORОNTO, ON
-M4T 1Y7
-647 786 4344 (MAIN NUMBER)
-4164744786
-TIMINGS:
-MONDAY - FRIDAY: 8AM - 8PM
-WЕEKENDS: 10AM - 7PM</t>
-  </si>
-  <si>
-    <t>Apple AirPods - AirPods Pro 2nd Gen, AirPods 2nd Gen, 3rd Gen</t>
-  </si>
-  <si>
-    <t>Samsung Tablets - Samsung Tab S9+, S9 FE, FE+, S9 Ultra, S6 Lite</t>
-  </si>
-  <si>
-    <t>Ecohouzng Tower Air Cooler with Humidity, 41-inches</t>
-  </si>
-  <si>
-    <t>Arctic King Window Air Conditioner 10000 BTU</t>
-  </si>
-  <si>
-    <t>Dyson Vacuums - Gen5 Outsize, Gen5 Detect, V15 Detect, DC77</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10000 BTU Air Conditioners - Arctic King, KoolKing </t>
   </si>
 </sst>
 </file>
@@ -13909,8 +13932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7C37E95-DA10-4114-8C3C-4F9671C16C16}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14022,7 +14045,7 @@
         <v>125</v>
       </c>
       <c r="D3" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
@@ -14154,7 +14177,7 @@
         <v>65</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
@@ -14482,7 +14505,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="B14" t="s">
         <v>494</v>
@@ -14490,8 +14513,8 @@
       <c r="C14">
         <v>325</v>
       </c>
-      <c r="D14" t="s">
-        <v>638</v>
+      <c r="D14" s="3" t="s">
+        <v>756</v>
       </c>
       <c r="E14" t="s">
         <v>14</v>
@@ -14532,7 +14555,7 @@
         <v>135</v>
       </c>
       <c r="D15" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="E15" t="s">
         <v>14</v>
@@ -14728,7 +14751,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B20" t="s">
         <v>494</v>
@@ -14737,7 +14760,7 @@
         <v>105</v>
       </c>
       <c r="D20" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="E20" t="s">
         <v>14</v>
@@ -14810,7 +14833,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="B22" t="s">
         <v>492</v>
@@ -14819,7 +14842,7 @@
         <v>120</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="E22" t="s">
         <v>14</v>
@@ -14851,7 +14874,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="B23" t="s">
         <v>497</v>
@@ -14860,7 +14883,7 @@
         <v>375</v>
       </c>
       <c r="D23" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="E23" t="s">
         <v>14</v>
@@ -15056,7 +15079,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B28" t="s">
         <v>499</v>
@@ -15065,7 +15088,7 @@
         <v>245</v>
       </c>
       <c r="D28" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="E28" t="s">
         <v>14</v>
@@ -15220,7 +15243,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B32" t="s">
         <v>491</v>
@@ -15229,13 +15252,13 @@
         <v>395</v>
       </c>
       <c r="D32" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="E32" t="s">
         <v>14</v>
       </c>
       <c r="H32" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="I32">
         <v>4164744786</v>
@@ -15264,7 +15287,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15550,7 +15573,7 @@
         <v>95</v>
       </c>
       <c r="D7" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
@@ -15835,7 +15858,7 @@
         <v>541</v>
       </c>
       <c r="K13" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="L13" t="s">
         <v>253</v>
@@ -15879,7 +15902,7 @@
         <v>545</v>
       </c>
       <c r="K14" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="L14" t="s">
         <v>253</v>
@@ -15923,7 +15946,7 @@
         <v>549</v>
       </c>
       <c r="K15" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="L15" t="s">
         <v>253</v>
@@ -16099,7 +16122,7 @@
         <v>567</v>
       </c>
       <c r="K19" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="L19" t="s">
         <v>253</v>
@@ -16143,7 +16166,7 @@
         <v>571</v>
       </c>
       <c r="K20" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="L20" t="s">
         <v>253</v>
@@ -16187,7 +16210,7 @@
         <v>575</v>
       </c>
       <c r="K21" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="L21" t="s">
         <v>253</v>
@@ -16231,7 +16254,7 @@
         <v>579</v>
       </c>
       <c r="K22" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="L22" t="s">
         <v>253</v>
@@ -16275,7 +16298,7 @@
         <v>579</v>
       </c>
       <c r="K23" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="L23" t="s">
         <v>253</v>
@@ -16319,7 +16342,7 @@
         <v>586</v>
       </c>
       <c r="K24" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="L24" t="s">
         <v>253</v>
@@ -16363,7 +16386,7 @@
         <v>590</v>
       </c>
       <c r="K25" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="L25" t="s">
         <v>253</v>
@@ -16377,7 +16400,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B26" t="s">
         <v>492</v>
@@ -16386,7 +16409,7 @@
         <v>125</v>
       </c>
       <c r="D26" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="E26" t="s">
         <v>14</v>
@@ -16398,16 +16421,16 @@
         <v>35</v>
       </c>
       <c r="H26" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="I26">
         <v>4164744786</v>
       </c>
       <c r="J26" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="K26" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="L26" t="s">
         <v>253</v>
@@ -16421,7 +16444,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B27" t="s">
         <v>497</v>
@@ -16430,7 +16453,7 @@
         <v>275</v>
       </c>
       <c r="D27" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="E27" t="s">
         <v>14</v>
@@ -16442,16 +16465,16 @@
         <v>35</v>
       </c>
       <c r="H27" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="I27">
         <v>4164744786</v>
       </c>
       <c r="J27" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="K27" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="L27" t="s">
         <v>253</v>
@@ -16465,7 +16488,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B28" t="s">
         <v>497</v>
@@ -16474,7 +16497,7 @@
         <v>245</v>
       </c>
       <c r="D28" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="E28" t="s">
         <v>14</v>
@@ -16486,16 +16509,16 @@
         <v>35</v>
       </c>
       <c r="H28" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="I28">
         <v>4164744786</v>
       </c>
       <c r="J28" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="K28" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="L28" t="s">
         <v>253</v>
@@ -16509,7 +16532,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B29" t="s">
         <v>497</v>
@@ -16518,7 +16541,7 @@
         <v>175</v>
       </c>
       <c r="D29" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="E29" t="s">
         <v>14</v>
@@ -16530,16 +16553,16 @@
         <v>35</v>
       </c>
       <c r="H29" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I29">
         <v>4164744786</v>
       </c>
       <c r="J29" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="K29" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="L29" t="s">
         <v>253</v>
@@ -16553,7 +16576,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B30" t="s">
         <v>497</v>
@@ -16562,7 +16585,7 @@
         <v>175</v>
       </c>
       <c r="D30" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="E30" t="s">
         <v>14</v>
@@ -16574,16 +16597,16 @@
         <v>35</v>
       </c>
       <c r="H30" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="I30">
         <v>4164744786</v>
       </c>
       <c r="J30" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="K30" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="L30" t="s">
         <v>253</v>
@@ -16597,7 +16620,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="B31" t="s">
         <v>498</v>
@@ -16606,7 +16629,7 @@
         <v>95</v>
       </c>
       <c r="D31" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="E31" t="s">
         <v>14</v>
@@ -16618,16 +16641,16 @@
         <v>35</v>
       </c>
       <c r="H31" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="I31">
         <v>4164744786</v>
       </c>
       <c r="J31" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="K31" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="L31" t="s">
         <v>253</v>
@@ -16904,7 +16927,7 @@
         <v>112</v>
       </c>
       <c r="M6" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="N6" t="s">
         <v>16</v>
@@ -16912,7 +16935,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B7" t="s">
         <v>499</v>
@@ -16921,7 +16944,7 @@
         <v>165</v>
       </c>
       <c r="D7" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
@@ -16962,7 +16985,7 @@
         <v>125</v>
       </c>
       <c r="D8" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -17126,7 +17149,7 @@
         <v>260</v>
       </c>
       <c r="D12" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="E12" t="s">
         <v>14</v>
@@ -17322,7 +17345,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="B17" t="s">
         <v>491</v>
@@ -17577,7 +17600,7 @@
         <v>95</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="E23" t="s">
         <v>14</v>
@@ -17788,7 +17811,7 @@
         <v>14</v>
       </c>
       <c r="F28" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="G28" t="s">
         <v>35</v>
@@ -17814,7 +17837,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B29" t="s">
         <v>499</v>
@@ -17823,7 +17846,7 @@
         <v>95</v>
       </c>
       <c r="D29" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E29" t="s">
         <v>14</v>
@@ -17896,7 +17919,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="B31" t="s">
         <v>498</v>
@@ -17905,7 +17928,7 @@
         <v>375</v>
       </c>
       <c r="D31" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="E31" t="s">
         <v>14</v>
@@ -17917,7 +17940,7 @@
         <v>35</v>
       </c>
       <c r="H31" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="I31">
         <v>4164744786</v>
@@ -18050,7 +18073,7 @@
         <v>65</v>
       </c>
       <c r="D3" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
@@ -18337,7 +18360,7 @@
         <v>195</v>
       </c>
       <c r="D10" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
@@ -18369,7 +18392,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B11" t="s">
         <v>603</v>
@@ -18378,7 +18401,7 @@
         <v>115</v>
       </c>
       <c r="D11" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E11" t="s">
         <v>14</v>
@@ -18738,7 +18761,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B20" t="s">
         <v>501</v>
@@ -18747,7 +18770,7 @@
         <v>275</v>
       </c>
       <c r="D20" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="E20" t="s">
         <v>14</v>
@@ -18911,7 +18934,7 @@
         <v>895</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="E24" t="s">
         <v>14</v>
@@ -19075,7 +19098,7 @@
         <v>100</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="E28" t="s">
         <v>14</v>
@@ -19271,7 +19294,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B33" t="s">
         <v>498</v>
@@ -19280,7 +19303,7 @@
         <v>375</v>
       </c>
       <c r="D33" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="E33" t="s">
         <v>14</v>
@@ -19319,8 +19342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7DC4EA-AA62-4FCC-9A5F-F63981EA274A}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19424,7 +19447,7 @@
         <v>695</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
@@ -19690,7 +19713,7 @@
         <v>375</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
@@ -19994,7 +20017,7 @@
         <v>85</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="E18" t="s">
         <v>14</v>
@@ -20108,7 +20131,7 @@
         <v>95</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="E21" t="s">
         <v>14</v>
@@ -20175,7 +20198,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B23" t="s">
         <v>497</v>
@@ -20184,13 +20207,13 @@
         <v>150</v>
       </c>
       <c r="D23" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="E23" t="s">
         <v>14</v>
       </c>
       <c r="F23" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="G23" t="s">
         <v>35</v>
@@ -20222,7 +20245,7 @@
         <v>190</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="E24" t="s">
         <v>14</v>
@@ -20251,7 +20274,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B25" t="s">
         <v>497</v>
@@ -20260,7 +20283,7 @@
         <v>55</v>
       </c>
       <c r="D25" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="E25" t="s">
         <v>14</v>
@@ -20441,7 +20464,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="B30" t="s">
         <v>498</v>
@@ -20450,7 +20473,7 @@
         <v>325</v>
       </c>
       <c r="D30" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="E30" t="s">
         <v>14</v>
@@ -20462,7 +20485,7 @@
         <v>35</v>
       </c>
       <c r="H30" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="I30">
         <v>6477864344</v>
@@ -20479,7 +20502,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="B31" t="s">
         <v>498</v>
@@ -20488,7 +20511,7 @@
         <v>395</v>
       </c>
       <c r="D31" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="E31" t="s">
         <v>14</v>
@@ -20500,7 +20523,7 @@
         <v>35</v>
       </c>
       <c r="H31" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="I31">
         <v>6477864344</v>
@@ -20517,7 +20540,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="B32" t="s">
         <v>609</v>
@@ -20526,7 +20549,7 @@
         <v>260</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="E32" t="s">
         <v>14</v>
@@ -20538,7 +20561,7 @@
         <v>35</v>
       </c>
       <c r="H32" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="I32">
         <v>6477864344</v>
@@ -20562,8 +20585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9AC7EE2-A1EB-433C-A565-CD8D185EEC9C}">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20621,7 +20644,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B2" t="s">
         <v>501</v>
@@ -20630,7 +20653,7 @@
         <v>250</v>
       </c>
       <c r="D2" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
@@ -20662,7 +20685,7 @@
         <v>250</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
@@ -20694,7 +20717,7 @@
         <v>275</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
@@ -20854,7 +20877,7 @@
         <v>225</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
@@ -20877,7 +20900,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="B10" t="s">
         <v>612</v>
@@ -20886,7 +20909,7 @@
         <v>75</v>
       </c>
       <c r="D10" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
@@ -20982,7 +21005,7 @@
         <v>295</v>
       </c>
       <c r="D13" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E13" t="s">
         <v>14</v>
@@ -21110,7 +21133,7 @@
         <v>225</v>
       </c>
       <c r="D17" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E17" t="s">
         <v>14</v>
@@ -21269,8 +21292,8 @@
       <c r="C22">
         <v>115</v>
       </c>
-      <c r="D22" t="s">
-        <v>693</v>
+      <c r="D22" s="3" t="s">
+        <v>757</v>
       </c>
       <c r="E22" t="s">
         <v>14</v>
@@ -21389,7 +21412,7 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B26" t="s">
         <v>501</v>
@@ -21398,7 +21421,7 @@
         <v>200</v>
       </c>
       <c r="D26" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="E26" t="s">
         <v>14</v>
@@ -21520,7 +21543,7 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="B30" t="s">
         <v>498</v>
@@ -21529,7 +21552,7 @@
         <v>495</v>
       </c>
       <c r="D30" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="E30" t="s">
         <v>14</v>
@@ -21541,7 +21564,7 @@
         <v>35</v>
       </c>
       <c r="H30" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="I30">
         <v>6477864344</v>
@@ -21552,7 +21575,7 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="B31" t="s">
         <v>501</v>
@@ -21561,7 +21584,7 @@
         <v>745</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="E31" t="s">
         <v>14</v>
@@ -21573,7 +21596,7 @@
         <v>35</v>
       </c>
       <c r="H31" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="I31">
         <v>6477864344</v>
@@ -21584,7 +21607,7 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="B32" t="s">
         <v>497</v>
@@ -21593,7 +21616,7 @@
         <v>975</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="E32" t="s">
         <v>14</v>
@@ -21605,7 +21628,7 @@
         <v>35</v>
       </c>
       <c r="H32" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="I32">
         <v>6477864344</v>
@@ -21623,7 +21646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11ECE094-2462-4974-B0F3-77B949CAF0B2}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -22353,7 +22376,7 @@
         <v>35</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="E21" t="s">
         <v>14</v>
@@ -22414,7 +22437,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B23" t="s">
         <v>499</v>

</xml_diff>